<commit_message>
pushing updated test files
</commit_message>
<xml_diff>
--- a/Tests/baseline_sma_5_25_JPM.xlsx
+++ b/Tests/baseline_sma_5_25_JPM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Windows\Documents\bt_plat\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9DCCF4-98C8-4C90-B4F1-708F5E077F8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB4461D-9785-44F6-B210-F0CE5C881A15}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,24 +29,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={A5D6C7E9-F67F-427A-95C4-3D4387A8DA0D}</author>
-  </authors>
-  <commentList>
-    <comment ref="J79" authorId="0" shapeId="0" xr:uid="{A5D6C7E9-F67F-427A-95C4-3D4387A8DA0D}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    modified from 130 (due to rounding)</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -157,14 +139,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -184,9 +165,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Biarys Saktaganov" id="{B3FF3C70-32A1-4576-B0D4-A983D710861F}" userId="65c7ae7bdea1f6d8" providerId="Windows Live"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -450,20 +429,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="J79" dT="2019-10-18T02:16:19.67" personId="{B3FF3C70-32A1-4576-B0D4-A983D710861F}" id="{A5D6C7E9-F67F-427A-95C4-3D4387A8DA0D}">
-    <text>modified from 130 (due to rounding)</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q287"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="X76" sqref="X76"/>
+    <sheetView topLeftCell="A252" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:Q287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4640,13 +4611,13 @@
       <c r="F79" s="4">
         <v>9.7100000000000009</v>
       </c>
-      <c r="G79" s="7">
+      <c r="G79" s="6">
         <v>0.22600000000000001</v>
       </c>
       <c r="H79" s="4">
         <v>232.7</v>
       </c>
-      <c r="I79" s="7">
+      <c r="I79" s="6">
         <v>0.22600000000000001</v>
       </c>
       <c r="J79" s="4">
@@ -4664,10 +4635,10 @@
       <c r="N79" s="4">
         <v>4.01</v>
       </c>
-      <c r="O79" s="7">
+      <c r="O79" s="6">
         <v>-3.1600000000000003E-2</v>
       </c>
-      <c r="P79" s="7">
+      <c r="P79" s="6">
         <v>0.35730000000000001</v>
       </c>
       <c r="Q79" s="4" t="s">
@@ -15704,11 +15675,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC41757A-AC97-41E0-ADEC-9FB26D7A223F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC41757A-AC97-41E0-ADEC-9FB26D7A223F}">
   <dimension ref="A1:P287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="I136" sqref="I136"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="G136" sqref="G136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15717,7 +15688,7 @@
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -15740,7 +15711,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -18861,29 +18832,29 @@
       <c r="E79" s="5">
         <v>32325</v>
       </c>
-      <c r="F79" s="6">
+      <c r="F79" s="4">
         <v>9.7100000000000009</v>
       </c>
-      <c r="G79" s="7">
+      <c r="G79" s="6">
         <v>0.22600000000000001</v>
       </c>
       <c r="H79" s="4">
-        <v>234.49</v>
-      </c>
-      <c r="I79" s="7">
+        <v>232.7</v>
+      </c>
+      <c r="I79" s="6">
         <v>0.22600000000000001</v>
       </c>
       <c r="J79" s="4">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K79" s="4">
-        <v>1037.52</v>
+        <v>1029.5999999999999</v>
       </c>
       <c r="L79" s="4">
-        <v>609.69000000000005</v>
-      </c>
-      <c r="O79" s="7"/>
-      <c r="P79" s="7"/>
+        <v>607.9</v>
+      </c>
+      <c r="O79" s="6"/>
+      <c r="P79" s="6"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
@@ -18901,7 +18872,7 @@
       <c r="E80" s="1">
         <v>32345</v>
       </c>
-      <c r="F80" s="3">
+      <c r="F80">
         <v>9.8800000000000008</v>
       </c>
       <c r="G80" s="2">
@@ -18920,7 +18891,7 @@
         <v>1057.32</v>
       </c>
       <c r="L80">
-        <v>619.41</v>
+        <v>617.62</v>
       </c>
       <c r="O80" s="2"/>
       <c r="P80" s="2"/>
@@ -18941,7 +18912,7 @@
       <c r="E81" s="1">
         <v>32385</v>
       </c>
-      <c r="F81" s="3">
+      <c r="F81">
         <v>10.63</v>
       </c>
       <c r="G81" s="2">
@@ -18960,7 +18931,7 @@
         <v>1056.46</v>
       </c>
       <c r="L81">
-        <v>636.58000000000004</v>
+        <v>634.79</v>
       </c>
       <c r="O81" s="2"/>
       <c r="P81" s="2"/>
@@ -18981,7 +18952,7 @@
       <c r="E82" s="1">
         <v>32400</v>
       </c>
-      <c r="F82" s="3">
+      <c r="F82">
         <v>10.58</v>
       </c>
       <c r="G82" s="2">
@@ -19000,7 +18971,7 @@
         <v>1056</v>
       </c>
       <c r="L82">
-        <v>596.26</v>
+        <v>594.47</v>
       </c>
       <c r="O82" s="2"/>
       <c r="P82" s="2"/>
@@ -19021,7 +18992,7 @@
       <c r="E83" s="1">
         <v>32414</v>
       </c>
-      <c r="F83" s="3">
+      <c r="F83">
         <v>10.63</v>
       </c>
       <c r="G83" s="2">
@@ -19040,7 +19011,7 @@
         <v>1055.3599999999999</v>
       </c>
       <c r="L83">
-        <v>572.01</v>
+        <v>570.22</v>
       </c>
       <c r="O83" s="2"/>
       <c r="P83" s="2"/>
@@ -19061,7 +19032,7 @@
       <c r="E84" s="1">
         <v>32490</v>
       </c>
-      <c r="F84" s="3">
+      <c r="F84">
         <v>10.38</v>
       </c>
       <c r="G84" s="2">
@@ -19080,7 +19051,7 @@
         <v>1049.58</v>
       </c>
       <c r="L84">
-        <v>539.66999999999996</v>
+        <v>537.88</v>
       </c>
       <c r="O84" s="2"/>
       <c r="P84" s="2"/>
@@ -19101,7 +19072,7 @@
       <c r="E85" s="1">
         <v>32554</v>
       </c>
-      <c r="F85" s="3">
+      <c r="F85">
         <v>10.63</v>
       </c>
       <c r="G85" s="2">
@@ -19120,7 +19091,7 @@
         <v>1047.42</v>
       </c>
       <c r="L85">
-        <v>544.62</v>
+        <v>542.83000000000004</v>
       </c>
       <c r="O85" s="2"/>
       <c r="P85" s="2"/>
@@ -19141,7 +19112,7 @@
       <c r="E86" s="1">
         <v>32633</v>
       </c>
-      <c r="F86" s="3">
+      <c r="F86">
         <v>11.5</v>
       </c>
       <c r="G86" s="2">
@@ -19160,7 +19131,7 @@
         <v>1049.97</v>
       </c>
       <c r="L86">
-        <v>564.15</v>
+        <v>562.36</v>
       </c>
       <c r="O86" s="2"/>
       <c r="P86" s="2"/>
@@ -19181,7 +19152,7 @@
       <c r="E87" s="1">
         <v>32674</v>
       </c>
-      <c r="F87" s="3">
+      <c r="F87">
         <v>11.58</v>
       </c>
       <c r="G87" s="2">
@@ -19200,7 +19171,7 @@
         <v>1050.3</v>
       </c>
       <c r="L87">
-        <v>556.04999999999995</v>
+        <v>554.26</v>
       </c>
       <c r="O87" s="2"/>
       <c r="P87" s="2"/>
@@ -19221,7 +19192,7 @@
       <c r="E88" s="1">
         <v>32695</v>
       </c>
-      <c r="F88" s="3">
+      <c r="F88">
         <v>12</v>
       </c>
       <c r="G88" s="2">
@@ -19240,7 +19211,7 @@
         <v>1052.48</v>
       </c>
       <c r="L88">
-        <v>559.57000000000005</v>
+        <v>557.78</v>
       </c>
       <c r="O88" s="2"/>
       <c r="P88" s="2"/>
@@ -19261,7 +19232,7 @@
       <c r="E89" s="1">
         <v>32741</v>
       </c>
-      <c r="F89" s="3">
+      <c r="F89">
         <v>12.42</v>
       </c>
       <c r="G89" s="2">
@@ -19280,7 +19251,7 @@
         <v>1046.6199999999999</v>
       </c>
       <c r="L89">
-        <v>581.07000000000005</v>
+        <v>579.28</v>
       </c>
       <c r="O89" s="2"/>
       <c r="P89" s="2"/>
@@ -19301,7 +19272,7 @@
       <c r="E90" s="1">
         <v>32797</v>
       </c>
-      <c r="F90" s="3">
+      <c r="F90">
         <v>12.29</v>
       </c>
       <c r="G90" s="2">
@@ -19320,7 +19291,7 @@
         <v>1050.4000000000001</v>
       </c>
       <c r="L90">
-        <v>513.87</v>
+        <v>512.08000000000004</v>
       </c>
       <c r="O90" s="2"/>
       <c r="P90" s="2"/>
@@ -19341,7 +19312,7 @@
       <c r="E91" s="1">
         <v>32853</v>
       </c>
-      <c r="F91" s="3">
+      <c r="F91">
         <v>10.75</v>
       </c>
       <c r="G91" s="2">
@@ -19360,7 +19331,7 @@
         <v>1050.51</v>
       </c>
       <c r="L91">
-        <v>506.11</v>
+        <v>504.32</v>
       </c>
       <c r="O91" s="2"/>
       <c r="P91" s="2"/>
@@ -19381,7 +19352,7 @@
       <c r="E92" s="1">
         <v>32884</v>
       </c>
-      <c r="F92" s="3">
+      <c r="F92">
         <v>9.92</v>
       </c>
       <c r="G92" s="2">
@@ -19400,7 +19371,7 @@
         <v>1042</v>
       </c>
       <c r="L92">
-        <v>456.11</v>
+        <v>454.32</v>
       </c>
       <c r="O92" s="2"/>
       <c r="P92" s="2"/>
@@ -19421,7 +19392,7 @@
       <c r="E93" s="1">
         <v>32951</v>
       </c>
-      <c r="F93" s="3">
+      <c r="F93">
         <v>8.6300000000000008</v>
       </c>
       <c r="G93" s="2">
@@ -19440,7 +19411,7 @@
         <v>1043.6400000000001</v>
       </c>
       <c r="L93">
-        <v>422.18</v>
+        <v>420.39</v>
       </c>
       <c r="O93" s="2"/>
       <c r="P93" s="2"/>
@@ -19461,7 +19432,7 @@
       <c r="E94" s="1">
         <v>32983</v>
       </c>
-      <c r="F94" s="3">
+      <c r="F94">
         <v>7.75</v>
       </c>
       <c r="G94" s="2">
@@ -19480,7 +19451,7 @@
         <v>1034.8</v>
       </c>
       <c r="L94">
-        <v>394.88</v>
+        <v>393.09</v>
       </c>
       <c r="O94" s="2"/>
       <c r="P94" s="2"/>
@@ -19501,7 +19472,7 @@
       <c r="E95" s="1">
         <v>32995</v>
       </c>
-      <c r="F95" s="3">
+      <c r="F95">
         <v>7.83</v>
       </c>
       <c r="G95" s="2">
@@ -19520,7 +19491,7 @@
         <v>1032.28</v>
       </c>
       <c r="L95">
-        <v>388.33</v>
+        <v>386.54</v>
       </c>
       <c r="O95" s="2"/>
       <c r="P95" s="2"/>
@@ -19541,7 +19512,7 @@
       <c r="E96" s="1">
         <v>33039</v>
       </c>
-      <c r="F96" s="3">
+      <c r="F96">
         <v>8.75</v>
       </c>
       <c r="G96" s="2">
@@ -19560,7 +19531,7 @@
         <v>1036.25</v>
       </c>
       <c r="L96">
-        <v>445.83</v>
+        <v>444.04</v>
       </c>
       <c r="O96" s="2"/>
       <c r="P96" s="2"/>
@@ -19581,7 +19552,7 @@
       <c r="E97" s="1">
         <v>33106</v>
       </c>
-      <c r="F97" s="3">
+      <c r="F97">
         <v>7.5</v>
       </c>
       <c r="G97" s="2">
@@ -19600,7 +19571,7 @@
         <v>1037.1600000000001</v>
       </c>
       <c r="L97">
-        <v>376.17</v>
+        <v>374.38</v>
       </c>
       <c r="O97" s="2"/>
       <c r="P97" s="2"/>
@@ -19621,7 +19592,7 @@
       <c r="E98" s="1">
         <v>33206</v>
       </c>
-      <c r="F98" s="3">
+      <c r="F98">
         <v>3.67</v>
       </c>
       <c r="G98" s="2">
@@ -19640,7 +19611,7 @@
         <v>1036</v>
       </c>
       <c r="L98">
-        <v>290.7</v>
+        <v>288.91000000000003</v>
       </c>
       <c r="O98" s="2"/>
       <c r="P98" s="2"/>
@@ -19661,7 +19632,7 @@
       <c r="E99" s="1">
         <v>33225</v>
       </c>
-      <c r="F99" s="3">
+      <c r="F99">
         <v>3.88</v>
       </c>
       <c r="G99" s="2">
@@ -19680,7 +19651,7 @@
         <v>1027.0899999999999</v>
       </c>
       <c r="L99">
-        <v>315.08999999999997</v>
+        <v>313.3</v>
       </c>
       <c r="O99" s="2"/>
       <c r="P99" s="2"/>
@@ -19701,7 +19672,7 @@
       <c r="E100" s="1">
         <v>33318</v>
       </c>
-      <c r="F100" s="3">
+      <c r="F100">
         <v>5.33</v>
       </c>
       <c r="G100" s="2">
@@ -19720,7 +19691,7 @@
         <v>1029.99</v>
       </c>
       <c r="L100">
-        <v>601.61</v>
+        <v>599.82000000000005</v>
       </c>
       <c r="O100" s="2"/>
       <c r="P100" s="2"/>
@@ -19741,7 +19712,7 @@
       <c r="E101" s="1">
         <v>33365</v>
       </c>
-      <c r="F101" s="3">
+      <c r="F101">
         <v>6.54</v>
       </c>
       <c r="G101" s="2">
@@ -19760,7 +19731,7 @@
         <v>1058.4000000000001</v>
       </c>
       <c r="L101">
-        <v>720.41</v>
+        <v>718.62</v>
       </c>
       <c r="O101" s="2"/>
       <c r="P101" s="2"/>
@@ -19781,7 +19752,7 @@
       <c r="E102" s="1">
         <v>33414</v>
       </c>
-      <c r="F102" s="3">
+      <c r="F102">
         <v>7.04</v>
       </c>
       <c r="G102" s="2">
@@ -19800,7 +19771,7 @@
         <v>1071</v>
       </c>
       <c r="L102">
-        <v>726.53</v>
+        <v>724.74</v>
       </c>
       <c r="O102" s="2"/>
       <c r="P102" s="2"/>
@@ -19821,7 +19792,7 @@
       <c r="E103" s="1">
         <v>33478</v>
       </c>
-      <c r="F103" s="3">
+      <c r="F103">
         <v>8.7100000000000009</v>
       </c>
       <c r="G103" s="2">
@@ -19840,7 +19811,7 @@
         <v>1069.2</v>
       </c>
       <c r="L103">
-        <v>833.18</v>
+        <v>831.39</v>
       </c>
       <c r="O103" s="2"/>
       <c r="P103" s="2"/>
@@ -19861,7 +19832,7 @@
       <c r="E104" s="1">
         <v>33536</v>
       </c>
-      <c r="F104" s="3">
+      <c r="F104">
         <v>8</v>
       </c>
       <c r="G104" s="2">
@@ -19880,7 +19851,7 @@
         <v>1077.7</v>
       </c>
       <c r="L104">
-        <v>795.48</v>
+        <v>793.69</v>
       </c>
       <c r="O104" s="2"/>
       <c r="P104" s="2"/>
@@ -19901,7 +19872,7 @@
       <c r="E105" s="1">
         <v>33557</v>
       </c>
-      <c r="F105" s="3">
+      <c r="F105">
         <v>7.96</v>
       </c>
       <c r="G105" s="2">
@@ -19920,7 +19891,7 @@
         <v>1072.5</v>
       </c>
       <c r="L105">
-        <v>757.78</v>
+        <v>755.99</v>
       </c>
       <c r="O105" s="2"/>
       <c r="P105" s="2"/>
@@ -19941,7 +19912,7 @@
       <c r="E106" s="1">
         <v>33673</v>
       </c>
-      <c r="F106" s="3">
+      <c r="F106">
         <v>10.79</v>
       </c>
       <c r="G106" s="2">
@@ -19960,7 +19931,7 @@
         <v>1070.68</v>
       </c>
       <c r="L106">
-        <v>1219.28</v>
+        <v>1217.49</v>
       </c>
       <c r="O106" s="2"/>
       <c r="P106" s="2"/>
@@ -19981,7 +19952,7 @@
       <c r="E107" s="1">
         <v>33696</v>
       </c>
-      <c r="F107" s="3">
+      <c r="F107">
         <v>10.5</v>
       </c>
       <c r="G107" s="2">
@@ -20000,7 +19971,7 @@
         <v>1119.3800000000001</v>
       </c>
       <c r="L107">
-        <v>1118.4000000000001</v>
+        <v>1116.6099999999999</v>
       </c>
       <c r="O107" s="2"/>
       <c r="P107" s="2"/>
@@ -20021,7 +19992,7 @@
       <c r="E108" s="1">
         <v>33751</v>
       </c>
-      <c r="F108" s="3">
+      <c r="F108">
         <v>12</v>
       </c>
       <c r="G108" s="2">
@@ -20040,7 +20011,7 @@
         <v>1107.74</v>
       </c>
       <c r="L108">
-        <v>1174.6600000000001</v>
+        <v>1172.8699999999999</v>
       </c>
       <c r="O108" s="2"/>
       <c r="P108" s="2"/>
@@ -20061,7 +20032,7 @@
       <c r="E109" s="1">
         <v>33772</v>
       </c>
-      <c r="F109" s="3">
+      <c r="F109">
         <v>11.63</v>
       </c>
       <c r="G109" s="2">
@@ -20080,7 +20051,7 @@
         <v>1114.96</v>
       </c>
       <c r="L109">
-        <v>1083.1400000000001</v>
+        <v>1081.3499999999999</v>
       </c>
       <c r="O109" s="2"/>
       <c r="P109" s="2"/>
@@ -20101,7 +20072,7 @@
       <c r="E110" s="1">
         <v>33802</v>
       </c>
-      <c r="F110" s="3">
+      <c r="F110">
         <v>11.96</v>
       </c>
       <c r="G110" s="2">
@@ -20120,7 +20091,7 @@
         <v>1098.81</v>
       </c>
       <c r="L110">
-        <v>1024.8499999999999</v>
+        <v>1023.06</v>
       </c>
       <c r="O110" s="2"/>
       <c r="P110" s="2"/>
@@ -20141,7 +20112,7 @@
       <c r="E111" s="1">
         <v>33886</v>
       </c>
-      <c r="F111" s="3">
+      <c r="F111">
         <v>10.33</v>
       </c>
       <c r="G111" s="2">
@@ -20160,7 +20131,7 @@
         <v>1092</v>
       </c>
       <c r="L111">
-        <v>965.85</v>
+        <v>964.06</v>
       </c>
       <c r="O111" s="2"/>
       <c r="P111" s="2"/>
@@ -20181,7 +20152,7 @@
       <c r="E112" s="1">
         <v>33890</v>
       </c>
-      <c r="F112" s="3">
+      <c r="F112">
         <v>10.54</v>
       </c>
       <c r="G112" s="2">
@@ -20200,7 +20171,7 @@
         <v>1089.74</v>
       </c>
       <c r="L112">
-        <v>961.73</v>
+        <v>959.94</v>
       </c>
       <c r="O112" s="2"/>
       <c r="P112" s="2"/>
@@ -20221,7 +20192,7 @@
       <c r="E113" s="1">
         <v>33952</v>
       </c>
-      <c r="F113" s="3">
+      <c r="F113">
         <v>12.08</v>
       </c>
       <c r="G113" s="2">
@@ -20240,7 +20211,7 @@
         <v>1087.8399999999999</v>
       </c>
       <c r="L113">
-        <v>1130.21</v>
+        <v>1128.42</v>
       </c>
       <c r="O113" s="2"/>
       <c r="P113" s="2"/>
@@ -20261,7 +20232,7 @@
       <c r="E114" s="1">
         <v>34018</v>
       </c>
-      <c r="F114" s="3">
+      <c r="F114">
         <v>13.25</v>
       </c>
       <c r="G114" s="2">
@@ -20280,7 +20251,7 @@
         <v>1107.04</v>
       </c>
       <c r="L114">
-        <v>1189.17</v>
+        <v>1187.3800000000001</v>
       </c>
       <c r="O114" s="2"/>
       <c r="P114" s="2"/>
@@ -20301,7 +20272,7 @@
       <c r="E115" s="1">
         <v>34029</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F115">
         <v>13.67</v>
       </c>
       <c r="G115" s="2">
@@ -20320,7 +20291,7 @@
         <v>1110.4000000000001</v>
       </c>
       <c r="L115">
-        <v>1172.3699999999999</v>
+        <v>1170.58</v>
       </c>
       <c r="O115" s="2"/>
       <c r="P115" s="2"/>
@@ -20341,7 +20312,7 @@
       <c r="E116" s="1">
         <v>34051</v>
       </c>
-      <c r="F116" s="3">
+      <c r="F116">
         <v>13.58</v>
       </c>
       <c r="G116" s="2">
@@ -20360,7 +20331,7 @@
         <v>1116.8</v>
       </c>
       <c r="L116">
-        <v>1141.97</v>
+        <v>1140.18</v>
       </c>
       <c r="O116" s="2"/>
       <c r="P116" s="2"/>
@@ -20381,7 +20352,7 @@
       <c r="E117" s="1">
         <v>34080</v>
       </c>
-      <c r="F117" s="3">
+      <c r="F117">
         <v>13.25</v>
       </c>
       <c r="G117" s="2">
@@ -20400,7 +20371,7 @@
         <v>1111.5</v>
       </c>
       <c r="L117">
-        <v>1063.97</v>
+        <v>1062.18</v>
       </c>
       <c r="O117" s="2"/>
       <c r="P117" s="2"/>
@@ -20421,7 +20392,7 @@
       <c r="E118" s="1">
         <v>34127</v>
       </c>
-      <c r="F118" s="3">
+      <c r="F118">
         <v>11.83</v>
       </c>
       <c r="G118" s="2">
@@ -20440,7 +20411,7 @@
         <v>1099.94</v>
       </c>
       <c r="L118">
-        <v>981.41</v>
+        <v>979.62</v>
       </c>
       <c r="O118" s="2"/>
       <c r="P118" s="2"/>
@@ -20461,7 +20432,7 @@
       <c r="E119" s="1">
         <v>34165</v>
       </c>
-      <c r="F119" s="3">
+      <c r="F119">
         <v>13.25</v>
       </c>
       <c r="G119" s="2">
@@ -20480,7 +20451,7 @@
         <v>1088.6400000000001</v>
       </c>
       <c r="L119">
-        <v>1005.77</v>
+        <v>1003.98</v>
       </c>
       <c r="O119" s="2"/>
       <c r="P119" s="2"/>
@@ -20501,7 +20472,7 @@
       <c r="E120" s="1">
         <v>34199</v>
       </c>
-      <c r="F120" s="3">
+      <c r="F120">
         <v>13.33</v>
       </c>
       <c r="G120" s="2">
@@ -20520,7 +20491,7 @@
         <v>1090.4000000000001</v>
       </c>
       <c r="L120">
-        <v>981.77</v>
+        <v>979.98</v>
       </c>
       <c r="O120" s="2"/>
       <c r="P120" s="2"/>
@@ -20541,7 +20512,7 @@
       <c r="E121" s="1">
         <v>34261</v>
       </c>
-      <c r="F121" s="3">
+      <c r="F121">
         <v>13.63</v>
       </c>
       <c r="G121" s="2">
@@ -20560,7 +20531,7 @@
         <v>1092.8800000000001</v>
       </c>
       <c r="L121">
-        <v>924.77</v>
+        <v>922.98</v>
       </c>
       <c r="O121" s="2"/>
       <c r="P121" s="2"/>
@@ -20581,7 +20552,7 @@
       <c r="E122" s="1">
         <v>34354</v>
       </c>
-      <c r="F122" s="3">
+      <c r="F122">
         <v>12.67</v>
       </c>
       <c r="G122" s="2">
@@ -20600,7 +20571,7 @@
         <v>1089.79</v>
       </c>
       <c r="L122">
-        <v>886.59</v>
+        <v>884.8</v>
       </c>
       <c r="O122" s="2"/>
       <c r="P122" s="2"/>
@@ -20621,7 +20592,7 @@
       <c r="E123" s="1">
         <v>34423</v>
       </c>
-      <c r="F123" s="3">
+      <c r="F123">
         <v>11.83</v>
       </c>
       <c r="G123" s="2">
@@ -20640,7 +20611,7 @@
         <v>1079</v>
       </c>
       <c r="L123">
-        <v>789.48</v>
+        <v>787.69</v>
       </c>
       <c r="O123" s="2"/>
       <c r="P123" s="2"/>
@@ -20661,7 +20632,7 @@
       <c r="E124" s="1">
         <v>34444</v>
       </c>
-      <c r="F124" s="3">
+      <c r="F124">
         <v>12.13</v>
       </c>
       <c r="G124" s="2">
@@ -20680,7 +20651,7 @@
         <v>1072.3599999999999</v>
       </c>
       <c r="L124">
-        <v>723.91</v>
+        <v>722.12</v>
       </c>
       <c r="O124" s="2"/>
       <c r="P124" s="2"/>
@@ -20701,7 +20672,7 @@
       <c r="E125" s="1">
         <v>34509</v>
       </c>
-      <c r="F125" s="3">
+      <c r="F125">
         <v>12.79</v>
       </c>
       <c r="G125" s="2">
@@ -20720,7 +20691,7 @@
         <v>1060.3800000000001</v>
       </c>
       <c r="L125">
-        <v>763.47</v>
+        <v>761.68</v>
       </c>
       <c r="O125" s="2"/>
       <c r="P125" s="2"/>
@@ -20741,7 +20712,7 @@
       <c r="E126" s="1">
         <v>34555</v>
       </c>
-      <c r="F126" s="3">
+      <c r="F126">
         <v>12.63</v>
       </c>
       <c r="G126" s="2">
@@ -20760,7 +20731,7 @@
         <v>1075.68</v>
       </c>
       <c r="L126">
-        <v>736.08</v>
+        <v>734.29</v>
       </c>
       <c r="O126" s="2"/>
       <c r="P126" s="2"/>
@@ -20781,7 +20752,7 @@
       <c r="E127" s="1">
         <v>34583</v>
       </c>
-      <c r="F127" s="3">
+      <c r="F127">
         <v>12.75</v>
       </c>
       <c r="G127" s="2">
@@ -20800,7 +20771,7 @@
         <v>1069.28</v>
       </c>
       <c r="L127">
-        <v>712.3</v>
+        <v>710.51</v>
       </c>
       <c r="O127" s="2"/>
       <c r="P127" s="2"/>
@@ -20821,7 +20792,7 @@
       <c r="E128" s="1">
         <v>34646</v>
       </c>
-      <c r="F128" s="3">
+      <c r="F128">
         <v>12.04</v>
       </c>
       <c r="G128" s="2">
@@ -20840,7 +20811,7 @@
         <v>1069.23</v>
       </c>
       <c r="L128">
-        <v>690.55</v>
+        <v>688.76</v>
       </c>
       <c r="O128" s="2"/>
       <c r="P128" s="2"/>
@@ -20861,7 +20832,7 @@
       <c r="E129" s="1">
         <v>34695</v>
       </c>
-      <c r="F129" s="3">
+      <c r="F129">
         <v>12.13</v>
       </c>
       <c r="G129" s="2">
@@ -20880,7 +20851,7 @@
         <v>1062.27</v>
       </c>
       <c r="L129">
-        <v>683.59</v>
+        <v>681.8</v>
       </c>
       <c r="O129" s="2"/>
       <c r="P129" s="2"/>
@@ -20901,7 +20872,7 @@
       <c r="E130" s="1">
         <v>34765</v>
       </c>
-      <c r="F130" s="3">
+      <c r="F130">
         <v>12.71</v>
       </c>
       <c r="G130" s="2">
@@ -20920,7 +20891,7 @@
         <v>1068.1199999999999</v>
       </c>
       <c r="L130">
-        <v>708.53</v>
+        <v>706.74</v>
       </c>
       <c r="O130" s="2"/>
       <c r="P130" s="2"/>
@@ -20941,7 +20912,7 @@
       <c r="E131" s="1">
         <v>34862</v>
       </c>
-      <c r="F131" s="3">
+      <c r="F131">
         <v>14.92</v>
       </c>
       <c r="G131" s="2">
@@ -20960,7 +20931,7 @@
         <v>1066.26</v>
       </c>
       <c r="L131">
-        <v>806.03</v>
+        <v>804.24</v>
       </c>
       <c r="O131" s="2"/>
       <c r="P131" s="2"/>
@@ -20981,7 +20952,7 @@
       <c r="E132" s="1">
         <v>34995</v>
       </c>
-      <c r="F132" s="3">
+      <c r="F132">
         <v>19.79</v>
       </c>
       <c r="G132" s="2">
@@ -21000,7 +20971,7 @@
         <v>1078.47</v>
       </c>
       <c r="L132">
-        <v>1093.07</v>
+        <v>1091.28</v>
       </c>
       <c r="O132" s="2"/>
       <c r="P132" s="2"/>
@@ -21021,7 +20992,7 @@
       <c r="E133" s="1">
         <v>35048</v>
       </c>
-      <c r="F133" s="3">
+      <c r="F133">
         <v>19.25</v>
       </c>
       <c r="G133" s="2">
@@ -21040,7 +21011,7 @@
         <v>1107.1500000000001</v>
       </c>
       <c r="L133">
-        <v>1044.67</v>
+        <v>1042.8800000000001</v>
       </c>
       <c r="O133" s="2"/>
       <c r="P133" s="2"/>
@@ -21061,7 +21032,7 @@
       <c r="E134" s="1">
         <v>35135</v>
       </c>
-      <c r="F134" s="3">
+      <c r="F134">
         <v>21.96</v>
       </c>
       <c r="G134" s="2">
@@ -21080,7 +21051,7 @@
         <v>1090.6500000000001</v>
       </c>
       <c r="L134">
-        <v>1161.82</v>
+        <v>1160.03</v>
       </c>
       <c r="O134" s="2"/>
       <c r="P134" s="2"/>
@@ -21101,7 +21072,7 @@
       <c r="E135" s="1">
         <v>35166</v>
       </c>
-      <c r="F135" s="3">
+      <c r="F135">
         <v>22.29</v>
       </c>
       <c r="G135" s="2">
@@ -21120,7 +21091,7 @@
         <v>1104</v>
       </c>
       <c r="L135">
-        <v>1083.1600000000001</v>
+        <v>1081.3699999999999</v>
       </c>
       <c r="O135" s="2"/>
       <c r="P135" s="2"/>
@@ -21141,7 +21112,7 @@
       <c r="E136" s="1">
         <v>35237</v>
       </c>
-      <c r="F136" s="3">
+      <c r="F136">
         <v>22.5</v>
       </c>
       <c r="G136" s="2">
@@ -21160,7 +21131,7 @@
         <v>1090.8699999999999</v>
       </c>
       <c r="L136">
-        <v>1049.79</v>
+        <v>1048</v>
       </c>
       <c r="O136" s="2"/>
       <c r="P136" s="2"/>
@@ -21181,7 +21152,7 @@
       <c r="E137" s="1">
         <v>35313</v>
       </c>
-      <c r="F137" s="3">
+      <c r="F137">
         <v>24.63</v>
       </c>
       <c r="G137" s="2">
@@ -21200,7 +21171,7 @@
         <v>1088.99</v>
       </c>
       <c r="L137">
-        <v>1118.4100000000001</v>
+        <v>1116.6199999999999</v>
       </c>
       <c r="O137" s="2"/>
       <c r="P137" s="2"/>
@@ -21221,7 +21192,7 @@
       <c r="E138" s="1">
         <v>35408</v>
       </c>
-      <c r="F138" s="3">
+      <c r="F138">
         <v>29.96</v>
       </c>
       <c r="G138" s="2">
@@ -21240,7 +21211,7 @@
         <v>1097.46</v>
       </c>
       <c r="L138">
-        <v>1279.27</v>
+        <v>1277.48</v>
       </c>
       <c r="O138" s="2"/>
       <c r="P138" s="2"/>
@@ -21261,7 +21232,7 @@
       <c r="E139" s="1">
         <v>35433</v>
       </c>
-      <c r="F139" s="3">
+      <c r="F139">
         <v>29.42</v>
       </c>
       <c r="G139" s="2">
@@ -21280,7 +21251,7 @@
         <v>1109.8800000000001</v>
       </c>
       <c r="L139">
-        <v>1228.51</v>
+        <v>1226.72</v>
       </c>
       <c r="O139" s="2"/>
       <c r="P139" s="2"/>
@@ -21301,7 +21272,7 @@
       <c r="E140" s="1">
         <v>35458</v>
       </c>
-      <c r="F140" s="3">
+      <c r="F140">
         <v>29.5</v>
       </c>
       <c r="G140" s="2">
@@ -21320,7 +21291,7 @@
         <v>1120.73</v>
       </c>
       <c r="L140">
-        <v>1199.28</v>
+        <v>1197.49</v>
       </c>
       <c r="O140" s="2"/>
       <c r="P140" s="2"/>
@@ -21341,7 +21312,7 @@
       <c r="E141" s="1">
         <v>35506</v>
       </c>
-      <c r="F141" s="3">
+      <c r="F141">
         <v>34.25</v>
       </c>
       <c r="G141" s="2">
@@ -21360,7 +21331,7 @@
         <v>1109.8800000000001</v>
       </c>
       <c r="L141">
-        <v>1322.4</v>
+        <v>1320.61</v>
       </c>
       <c r="O141" s="2"/>
       <c r="P141" s="2"/>
@@ -21381,7 +21352,7 @@
       <c r="E142" s="1">
         <v>35579</v>
       </c>
-      <c r="F142" s="3">
+      <c r="F142">
         <v>30.96</v>
       </c>
       <c r="G142" s="2">
@@ -21400,7 +21371,7 @@
         <v>1112.6500000000001</v>
       </c>
       <c r="L142">
-        <v>1293.3499999999999</v>
+        <v>1291.56</v>
       </c>
       <c r="O142" s="2"/>
       <c r="P142" s="2"/>
@@ -21421,7 +21392,7 @@
       <c r="E143" s="1">
         <v>35612</v>
       </c>
-      <c r="F143" s="3">
+      <c r="F143">
         <v>33.17</v>
       </c>
       <c r="G143" s="2">
@@ -21440,7 +21411,7 @@
         <v>1105</v>
       </c>
       <c r="L143">
-        <v>1316.13</v>
+        <v>1314.34</v>
       </c>
       <c r="O143" s="2"/>
       <c r="P143" s="2"/>
@@ -21461,7 +21432,7 @@
       <c r="E144" s="1">
         <v>35731</v>
       </c>
-      <c r="F144" s="3">
+      <c r="F144">
         <v>39.94</v>
       </c>
       <c r="G144" s="2">
@@ -21480,7 +21451,7 @@
         <v>1101.44</v>
       </c>
       <c r="L144">
-        <v>1492.77</v>
+        <v>1490.98</v>
       </c>
       <c r="O144" s="2"/>
       <c r="P144" s="2"/>
@@ -21501,7 +21472,7 @@
       <c r="E145" s="1">
         <v>35780</v>
       </c>
-      <c r="F145" s="3">
+      <c r="F145">
         <v>36.96</v>
       </c>
       <c r="G145" s="2">
@@ -21520,7 +21491,7 @@
         <v>1128.68</v>
       </c>
       <c r="L145">
-        <v>1435.93</v>
+        <v>1434.14</v>
       </c>
       <c r="O145" s="2"/>
       <c r="P145" s="2"/>
@@ -21541,7 +21512,7 @@
       <c r="E146" s="1">
         <v>35906</v>
       </c>
-      <c r="F146" s="3">
+      <c r="F146">
         <v>46.38</v>
       </c>
       <c r="G146" s="2">
@@ -21560,7 +21531,7 @@
         <v>1111.8</v>
       </c>
       <c r="L146">
-        <v>1715.53</v>
+        <v>1713.74</v>
       </c>
       <c r="O146" s="2"/>
       <c r="P146" s="2"/>
@@ -21581,7 +21552,7 @@
       <c r="E147" s="1">
         <v>35944</v>
       </c>
-      <c r="F147" s="3">
+      <c r="F147">
         <v>45.31</v>
       </c>
       <c r="G147" s="2">
@@ -21600,7 +21571,7 @@
         <v>1162.5</v>
       </c>
       <c r="L147">
-        <v>1685.78</v>
+        <v>1683.99</v>
       </c>
       <c r="O147" s="2"/>
       <c r="P147" s="2"/>
@@ -21621,7 +21592,7 @@
       <c r="E148" s="1">
         <v>35962</v>
       </c>
-      <c r="F148" s="3">
+      <c r="F148">
         <v>45.17</v>
       </c>
       <c r="G148" s="2">
@@ -21640,7 +21611,7 @@
         <v>1132.56</v>
       </c>
       <c r="L148">
-        <v>1637.3</v>
+        <v>1635.51</v>
       </c>
       <c r="O148" s="2"/>
       <c r="P148" s="2"/>
@@ -21661,7 +21632,7 @@
       <c r="E149" s="1">
         <v>35999</v>
       </c>
-      <c r="F149" s="3">
+      <c r="F149">
         <v>48.75</v>
       </c>
       <c r="G149" s="2">
@@ -21680,7 +21651,7 @@
         <v>1122.96</v>
       </c>
       <c r="L149">
-        <v>1684.34</v>
+        <v>1682.55</v>
       </c>
       <c r="O149" s="2"/>
       <c r="P149" s="2"/>
@@ -21701,7 +21672,7 @@
       <c r="E150" s="1">
         <v>36144</v>
       </c>
-      <c r="F150" s="3">
+      <c r="F150">
         <v>40.5</v>
       </c>
       <c r="G150" s="2">
@@ -21720,7 +21691,7 @@
         <v>1161.78</v>
       </c>
       <c r="L150">
-        <v>1899.56</v>
+        <v>1897.77</v>
       </c>
       <c r="O150" s="2"/>
       <c r="P150" s="2"/>
@@ -21741,7 +21712,7 @@
       <c r="E151" s="1">
         <v>36201</v>
       </c>
-      <c r="F151" s="3">
+      <c r="F151">
         <v>48.71</v>
       </c>
       <c r="G151" s="2">
@@ -21760,7 +21731,7 @@
         <v>1164.5</v>
       </c>
       <c r="L151">
-        <v>1952.81</v>
+        <v>1951.02</v>
       </c>
       <c r="O151" s="2"/>
       <c r="P151" s="2"/>
@@ -21781,7 +21752,7 @@
       <c r="E152" s="1">
         <v>36242</v>
       </c>
-      <c r="F152" s="3">
+      <c r="F152">
         <v>53.04</v>
       </c>
       <c r="G152" s="2">
@@ -21800,7 +21771,7 @@
         <v>1184.5</v>
       </c>
       <c r="L152">
-        <v>1988.23</v>
+        <v>1986.44</v>
       </c>
       <c r="O152" s="2"/>
       <c r="P152" s="2"/>
@@ -21821,7 +21792,7 @@
       <c r="E153" s="1">
         <v>36280</v>
       </c>
-      <c r="F153" s="3">
+      <c r="F153">
         <v>55</v>
       </c>
       <c r="G153" s="2">
@@ -21840,7 +21811,7 @@
         <v>1158.4000000000001</v>
       </c>
       <c r="L153">
-        <v>1929.83</v>
+        <v>1928.04</v>
       </c>
       <c r="O153" s="2"/>
       <c r="P153" s="2"/>
@@ -21861,7 +21832,7 @@
       <c r="E154" s="1">
         <v>36360</v>
       </c>
-      <c r="F154" s="3">
+      <c r="F154">
         <v>54.75</v>
       </c>
       <c r="G154" s="2">
@@ -21880,7 +21851,7 @@
         <v>1165.1199999999999</v>
       </c>
       <c r="L154">
-        <v>1969.21</v>
+        <v>1967.42</v>
       </c>
       <c r="O154" s="2"/>
       <c r="P154" s="2"/>
@@ -21901,7 +21872,7 @@
       <c r="E155" s="1">
         <v>36413</v>
       </c>
-      <c r="F155" s="3">
+      <c r="F155">
         <v>51.63</v>
       </c>
       <c r="G155" s="2">
@@ -21920,7 +21891,7 @@
         <v>1190.07</v>
       </c>
       <c r="L155">
-        <v>1863.37</v>
+        <v>1861.58</v>
       </c>
       <c r="O155" s="2"/>
       <c r="P155" s="2"/>
@@ -21941,7 +21912,7 @@
       <c r="E156" s="1">
         <v>36487</v>
       </c>
-      <c r="F156" s="3">
+      <c r="F156">
         <v>53.25</v>
       </c>
       <c r="G156" s="2">
@@ -21960,7 +21931,7 @@
         <v>1182.5</v>
       </c>
       <c r="L156">
-        <v>1852.37</v>
+        <v>1850.58</v>
       </c>
       <c r="O156" s="2"/>
       <c r="P156" s="2"/>
@@ -21981,7 +21952,7 @@
       <c r="E157" s="1">
         <v>36528</v>
       </c>
-      <c r="F157" s="3">
+      <c r="F157">
         <v>48.67</v>
       </c>
       <c r="G157" s="2">
@@ -22000,7 +21971,7 @@
         <v>1144.8800000000001</v>
       </c>
       <c r="L157">
-        <v>1778.23</v>
+        <v>1776.44</v>
       </c>
       <c r="O157" s="2"/>
       <c r="P157" s="2"/>
@@ -22021,7 +21992,7 @@
       <c r="E158" s="1">
         <v>36574</v>
       </c>
-      <c r="F158" s="3">
+      <c r="F158">
         <v>49.83</v>
       </c>
       <c r="G158" s="2">
@@ -22040,7 +22011,7 @@
         <v>1146.8599999999999</v>
       </c>
       <c r="L158">
-        <v>1727.63</v>
+        <v>1725.84</v>
       </c>
       <c r="O158" s="2"/>
       <c r="P158" s="2"/>
@@ -22061,7 +22032,7 @@
       <c r="E159" s="1">
         <v>36599</v>
       </c>
-      <c r="F159" s="3">
+      <c r="F159">
         <v>52.67</v>
       </c>
       <c r="G159" s="2">
@@ -22080,7 +22051,7 @@
         <v>1135.68</v>
       </c>
       <c r="L159">
-        <v>1698.02</v>
+        <v>1696.23</v>
       </c>
       <c r="O159" s="2"/>
       <c r="P159" s="2"/>
@@ -22101,7 +22072,7 @@
       <c r="E160" s="1">
         <v>36626</v>
       </c>
-      <c r="F160" s="3">
+      <c r="F160">
         <v>58.75</v>
       </c>
       <c r="G160" s="2">
@@ -22120,7 +22091,7 @@
         <v>1163.82</v>
       </c>
       <c r="L160">
-        <v>1767.95</v>
+        <v>1766.16</v>
       </c>
       <c r="O160" s="2"/>
       <c r="P160" s="2"/>
@@ -22141,7 +22112,7 @@
       <c r="E161" s="1">
         <v>36692</v>
       </c>
-      <c r="F161" s="3">
+      <c r="F161">
         <v>47.5</v>
       </c>
       <c r="G161" s="2">
@@ -22160,7 +22131,7 @@
         <v>1131.24</v>
       </c>
       <c r="L161">
-        <v>1681.71</v>
+        <v>1679.92</v>
       </c>
       <c r="O161" s="2"/>
       <c r="P161" s="2"/>
@@ -22181,7 +22152,7 @@
       <c r="E162" s="1">
         <v>36738</v>
       </c>
-      <c r="F162" s="3">
+      <c r="F162">
         <v>49.69</v>
       </c>
       <c r="G162" s="2">
@@ -22200,7 +22171,7 @@
         <v>1144.25</v>
       </c>
       <c r="L162">
-        <v>1680.33</v>
+        <v>1678.54</v>
       </c>
       <c r="O162" s="2"/>
       <c r="P162" s="2"/>
@@ -22221,7 +22192,7 @@
       <c r="E163" s="1">
         <v>36756</v>
       </c>
-      <c r="F163" s="3">
+      <c r="F163">
         <v>50.69</v>
       </c>
       <c r="G163" s="2">
@@ -22240,7 +22211,7 @@
         <v>1131.68</v>
       </c>
       <c r="L163">
-        <v>1663.83</v>
+        <v>1662.04</v>
       </c>
       <c r="O163" s="2"/>
       <c r="P163" s="2"/>
@@ -22261,7 +22232,7 @@
       <c r="E164" s="1">
         <v>36784</v>
       </c>
-      <c r="F164" s="3">
+      <c r="F164">
         <v>49.13</v>
       </c>
       <c r="G164" s="2">
@@ -22280,7 +22251,7 @@
         <v>1120.98</v>
       </c>
       <c r="L164">
-        <v>1574.58</v>
+        <v>1572.79</v>
       </c>
       <c r="O164" s="2"/>
       <c r="P164" s="2"/>
@@ -22301,7 +22272,7 @@
       <c r="E165" s="1">
         <v>36847</v>
       </c>
-      <c r="F165" s="3">
+      <c r="F165">
         <v>39.630000000000003</v>
       </c>
       <c r="G165" s="2">
@@ -22320,7 +22291,7 @@
         <v>1137.5</v>
       </c>
       <c r="L165">
-        <v>1427.83</v>
+        <v>1426.04</v>
       </c>
       <c r="O165" s="2"/>
       <c r="P165" s="2"/>
@@ -22341,7 +22312,7 @@
       <c r="E166" s="1">
         <v>36931</v>
       </c>
-      <c r="F166" s="3">
+      <c r="F166">
         <v>51.95</v>
       </c>
       <c r="G166" s="2">
@@ -22360,7 +22331,7 @@
         <v>1105</v>
       </c>
       <c r="L166">
-        <v>1673.53</v>
+        <v>1671.74</v>
       </c>
       <c r="O166" s="2"/>
       <c r="P166" s="2"/>
@@ -22381,7 +22352,7 @@
       <c r="E167" s="1">
         <v>37026</v>
       </c>
-      <c r="F167" s="3">
+      <c r="F167">
         <v>47.28</v>
       </c>
       <c r="G167" s="2">
@@ -22400,7 +22371,7 @@
         <v>1137.5</v>
       </c>
       <c r="L167">
-        <v>1718.03</v>
+        <v>1716.24</v>
       </c>
       <c r="O167" s="2"/>
       <c r="P167" s="2"/>
@@ -22421,7 +22392,7 @@
       <c r="E168" s="1">
         <v>37049</v>
       </c>
-      <c r="F168" s="3">
+      <c r="F168">
         <v>45.63</v>
       </c>
       <c r="G168" s="2">
@@ -22440,7 +22411,7 @@
         <v>1136.8900000000001</v>
       </c>
       <c r="L168">
-        <v>1630.63</v>
+        <v>1628.84</v>
       </c>
       <c r="O168" s="2"/>
       <c r="P168" s="2"/>
@@ -22461,7 +22432,7 @@
       <c r="E169" s="1">
         <v>37109</v>
       </c>
-      <c r="F169" s="3">
+      <c r="F169">
         <v>42.76</v>
       </c>
       <c r="G169" s="2">
@@ -22480,7 +22451,7 @@
         <v>1131</v>
       </c>
       <c r="L169">
-        <v>1611.39</v>
+        <v>1609.6</v>
       </c>
       <c r="O169" s="2"/>
       <c r="P169" s="2"/>
@@ -22501,7 +22472,7 @@
       <c r="E170" s="1">
         <v>37228</v>
       </c>
-      <c r="F170" s="3">
+      <c r="F170">
         <v>36.549999999999997</v>
       </c>
       <c r="G170" s="2">
@@ -22520,7 +22491,7 @@
         <v>1160.76</v>
       </c>
       <c r="L170">
-        <v>1693.33</v>
+        <v>1691.54</v>
       </c>
       <c r="O170" s="2"/>
       <c r="P170" s="2"/>
@@ -22541,7 +22512,7 @@
       <c r="E171" s="1">
         <v>37238</v>
       </c>
-      <c r="F171" s="3">
+      <c r="F171">
         <v>37.090000000000003</v>
       </c>
       <c r="G171" s="2">
@@ -22560,7 +22531,7 @@
         <v>1160.4000000000001</v>
       </c>
       <c r="L171">
-        <v>1645.63</v>
+        <v>1643.84</v>
       </c>
       <c r="O171" s="2"/>
       <c r="P171" s="2"/>
@@ -22581,7 +22552,7 @@
       <c r="E172" s="1">
         <v>37274</v>
       </c>
-      <c r="F172" s="3">
+      <c r="F172">
         <v>35.909999999999997</v>
       </c>
       <c r="G172" s="2">
@@ -22600,7 +22571,7 @@
         <v>1128.0999999999999</v>
       </c>
       <c r="L172">
-        <v>1558.92</v>
+        <v>1557.13</v>
       </c>
       <c r="O172" s="2"/>
       <c r="P172" s="2"/>
@@ -22621,7 +22592,7 @@
       <c r="E173" s="1">
         <v>37354</v>
       </c>
-      <c r="F173" s="3">
+      <c r="F173">
         <v>34.979999999999997</v>
       </c>
       <c r="G173" s="2">
@@ -22640,7 +22611,7 @@
         <v>1137.8499999999999</v>
       </c>
       <c r="L173">
-        <v>1645.37</v>
+        <v>1643.58</v>
       </c>
       <c r="O173" s="2"/>
       <c r="P173" s="2"/>
@@ -22661,7 +22632,7 @@
       <c r="E174" s="1">
         <v>37375</v>
       </c>
-      <c r="F174" s="3">
+      <c r="F174">
         <v>34.340000000000003</v>
       </c>
       <c r="G174" s="2">
@@ -22680,7 +22651,7 @@
         <v>1155.06</v>
       </c>
       <c r="L174">
-        <v>1554.85</v>
+        <v>1553.06</v>
       </c>
       <c r="O174" s="2"/>
       <c r="P174" s="2"/>
@@ -22701,7 +22672,7 @@
       <c r="E175" s="1">
         <v>37385</v>
       </c>
-      <c r="F175" s="3">
+      <c r="F175">
         <v>35.770000000000003</v>
       </c>
       <c r="G175" s="2">
@@ -22720,7 +22691,7 @@
         <v>1144.21</v>
       </c>
       <c r="L175">
-        <v>1519.51</v>
+        <v>1517.72</v>
       </c>
       <c r="O175" s="2"/>
       <c r="P175" s="2"/>
@@ -22741,7 +22712,7 @@
       <c r="E176" s="1">
         <v>37410</v>
       </c>
-      <c r="F176" s="3">
+      <c r="F176">
         <v>34.659999999999997</v>
       </c>
       <c r="G176" s="2">
@@ -22760,7 +22731,7 @@
         <v>1126.54</v>
       </c>
       <c r="L176">
-        <v>1467.43</v>
+        <v>1465.64</v>
       </c>
       <c r="O176" s="2"/>
       <c r="P176" s="2"/>
@@ -22781,7 +22752,7 @@
       <c r="E177" s="1">
         <v>37484</v>
       </c>
-      <c r="F177" s="3">
+      <c r="F177">
         <v>24.86</v>
       </c>
       <c r="G177" s="2">
@@ -22800,7 +22771,7 @@
         <v>1131.3</v>
       </c>
       <c r="L177">
-        <v>1454.83</v>
+        <v>1453.04</v>
       </c>
       <c r="O177" s="2"/>
       <c r="P177" s="2"/>
@@ -22821,7 +22792,7 @@
       <c r="E178" s="1">
         <v>37505</v>
       </c>
-      <c r="F178" s="3">
+      <c r="F178">
         <v>23.91</v>
       </c>
       <c r="G178" s="2">
@@ -22840,7 +22811,7 @@
         <v>1142.82</v>
       </c>
       <c r="L178">
-        <v>1316.23</v>
+        <v>1314.44</v>
       </c>
       <c r="O178" s="2"/>
       <c r="P178" s="2"/>
@@ -22861,7 +22832,7 @@
       <c r="E179" s="1">
         <v>37614</v>
       </c>
-      <c r="F179" s="3">
+      <c r="F179">
         <v>24.2</v>
       </c>
       <c r="G179" s="2">
@@ -22880,7 +22851,7 @@
         <v>1114.8499999999999</v>
       </c>
       <c r="L179">
-        <v>1532.38</v>
+        <v>1530.59</v>
       </c>
       <c r="O179" s="2"/>
       <c r="P179" s="2"/>
@@ -22901,7 +22872,7 @@
       <c r="E180" s="1">
         <v>37645</v>
       </c>
-      <c r="F180" s="3">
+      <c r="F180">
         <v>23.81</v>
       </c>
       <c r="G180" s="2">
@@ -22920,7 +22891,7 @@
         <v>1141.3599999999999</v>
       </c>
       <c r="L180">
-        <v>1438.66</v>
+        <v>1436.87</v>
       </c>
       <c r="O180" s="2"/>
       <c r="P180" s="2"/>
@@ -22941,7 +22912,7 @@
       <c r="E181" s="1">
         <v>37690</v>
       </c>
-      <c r="F181" s="3">
+      <c r="F181">
         <v>21.44</v>
       </c>
       <c r="G181" s="2">
@@ -22960,7 +22931,7 @@
         <v>1142.5</v>
       </c>
       <c r="L181">
-        <v>1368.16</v>
+        <v>1366.37</v>
       </c>
       <c r="O181" s="2"/>
       <c r="P181" s="2"/>
@@ -22981,7 +22952,7 @@
       <c r="E182" s="1">
         <v>37802</v>
       </c>
-      <c r="F182" s="3">
+      <c r="F182">
         <v>34.18</v>
       </c>
       <c r="G182" s="2">
@@ -23000,7 +22971,7 @@
         <v>1119.8399999999999</v>
       </c>
       <c r="L182">
-        <v>1888.96</v>
+        <v>1887.17</v>
       </c>
       <c r="O182" s="2"/>
       <c r="P182" s="2"/>
@@ -23021,7 +22992,7 @@
       <c r="E183" s="1">
         <v>37825</v>
       </c>
-      <c r="F183" s="3">
+      <c r="F183">
         <v>34.86</v>
       </c>
       <c r="G183" s="2">
@@ -23040,7 +23011,7 @@
         <v>1168.2</v>
       </c>
       <c r="L183">
-        <v>1871.14</v>
+        <v>1869.35</v>
       </c>
       <c r="O183" s="2"/>
       <c r="P183" s="2"/>
@@ -23061,7 +23032,7 @@
       <c r="E184" s="1">
         <v>37834</v>
       </c>
-      <c r="F184" s="3">
+      <c r="F184">
         <v>33.36</v>
       </c>
       <c r="G184" s="2">
@@ -23080,7 +23051,7 @@
         <v>1171.17</v>
       </c>
       <c r="L184">
-        <v>1800.85</v>
+        <v>1799.06</v>
       </c>
       <c r="O184" s="2"/>
       <c r="P184" s="2"/>
@@ -23101,7 +23072,7 @@
       <c r="E185" s="1">
         <v>37860</v>
       </c>
-      <c r="F185" s="3">
+      <c r="F185">
         <v>33.26</v>
       </c>
       <c r="G185" s="2">
@@ -23120,7 +23091,7 @@
         <v>1176.4000000000001</v>
       </c>
       <c r="L185">
-        <v>1755.29</v>
+        <v>1753.5</v>
       </c>
       <c r="O185" s="2"/>
       <c r="P185" s="2"/>
@@ -23141,7 +23112,7 @@
       <c r="E186" s="1">
         <v>37879</v>
       </c>
-      <c r="F186" s="3">
+      <c r="F186">
         <v>33.97</v>
       </c>
       <c r="G186" s="2">
@@ -23160,7 +23131,7 @@
         <v>1145.0999999999999</v>
       </c>
       <c r="L186">
-        <v>1731.2</v>
+        <v>1729.41</v>
       </c>
       <c r="O186" s="2"/>
       <c r="P186" s="2"/>
@@ -23181,7 +23152,7 @@
       <c r="E187" s="1">
         <v>37921</v>
       </c>
-      <c r="F187" s="3">
+      <c r="F187">
         <v>34.950000000000003</v>
       </c>
       <c r="G187" s="2">
@@ -23200,7 +23171,7 @@
         <v>1143.78</v>
       </c>
       <c r="L187">
-        <v>1740.77</v>
+        <v>1738.98</v>
       </c>
       <c r="O187" s="2"/>
       <c r="P187" s="2"/>
@@ -23221,7 +23192,7 @@
       <c r="E188" s="1">
         <v>37938</v>
       </c>
-      <c r="F188" s="3">
+      <c r="F188">
         <v>35.86</v>
       </c>
       <c r="G188" s="2">
@@ -23240,7 +23211,7 @@
         <v>1138.01</v>
       </c>
       <c r="L188">
-        <v>1714.42</v>
+        <v>1712.63</v>
       </c>
       <c r="O188" s="2"/>
       <c r="P188" s="2"/>
@@ -23261,7 +23232,7 @@
       <c r="E189" s="1">
         <v>38070</v>
       </c>
-      <c r="F189" s="3">
+      <c r="F189">
         <v>40.74</v>
       </c>
       <c r="G189" s="2">
@@ -23280,7 +23251,7 @@
         <v>1141.1199999999999</v>
       </c>
       <c r="L189">
-        <v>1876.98</v>
+        <v>1875.19</v>
       </c>
       <c r="O189" s="2"/>
       <c r="P189" s="2"/>
@@ -23301,7 +23272,7 @@
       <c r="E190" s="1">
         <v>38084</v>
       </c>
-      <c r="F190" s="3">
+      <c r="F190">
         <v>41.37</v>
       </c>
       <c r="G190" s="2">
@@ -23320,7 +23291,7 @@
         <v>1174.5999999999999</v>
       </c>
       <c r="L190">
-        <v>1860.74</v>
+        <v>1858.95</v>
       </c>
       <c r="O190" s="2"/>
       <c r="P190" s="2"/>
@@ -23341,7 +23312,7 @@
       <c r="E191" s="1">
         <v>38176</v>
       </c>
-      <c r="F191" s="3">
+      <c r="F191">
         <v>36.75</v>
       </c>
       <c r="G191" s="2">
@@ -23360,7 +23331,7 @@
         <v>1179.2</v>
       </c>
       <c r="L191">
-        <v>1857.54</v>
+        <v>1855.75</v>
       </c>
       <c r="O191" s="2"/>
       <c r="P191" s="2"/>
@@ -23381,7 +23352,7 @@
       <c r="E192" s="1">
         <v>38208</v>
       </c>
-      <c r="F192" s="3">
+      <c r="F192">
         <v>36.07</v>
       </c>
       <c r="G192" s="2">
@@ -23400,7 +23371,7 @@
         <v>1159.71</v>
       </c>
       <c r="L192">
-        <v>1816</v>
+        <v>1814.21</v>
       </c>
       <c r="O192" s="2"/>
       <c r="P192" s="2"/>
@@ -23421,7 +23392,7 @@
       <c r="E193" s="1">
         <v>38259</v>
       </c>
-      <c r="F193" s="3">
+      <c r="F193">
         <v>39.68</v>
       </c>
       <c r="G193" s="2">
@@ -23440,7 +23411,7 @@
         <v>1179.8399999999999</v>
       </c>
       <c r="L193">
-        <v>1905.92</v>
+        <v>1904.13</v>
       </c>
       <c r="O193" s="2"/>
       <c r="P193" s="2"/>
@@ -23461,7 +23432,7 @@
       <c r="E194" s="1">
         <v>38268</v>
       </c>
-      <c r="F194" s="3">
+      <c r="F194">
         <v>39.65</v>
       </c>
       <c r="G194" s="2">
@@ -23480,7 +23451,7 @@
         <v>1169.8599999999999</v>
       </c>
       <c r="L194">
-        <v>1885.91</v>
+        <v>1884.12</v>
       </c>
       <c r="O194" s="2"/>
       <c r="P194" s="2"/>
@@ -23501,7 +23472,7 @@
       <c r="E195" s="1">
         <v>38310</v>
       </c>
-      <c r="F195" s="3">
+      <c r="F195">
         <v>37.42</v>
       </c>
       <c r="G195" s="2">
@@ -23520,7 +23491,7 @@
         <v>1149.56</v>
       </c>
       <c r="L195">
-        <v>1821.53</v>
+        <v>1819.74</v>
       </c>
       <c r="O195" s="2"/>
       <c r="P195" s="2"/>
@@ -23541,7 +23512,7 @@
       <c r="E196" s="1">
         <v>38362</v>
       </c>
-      <c r="F196" s="3">
+      <c r="F196">
         <v>38.270000000000003</v>
       </c>
       <c r="G196" s="2">
@@ -23560,7 +23531,7 @@
         <v>1170.9000000000001</v>
       </c>
       <c r="L196">
-        <v>1798.73</v>
+        <v>1796.94</v>
       </c>
       <c r="O196" s="2"/>
       <c r="P196" s="2"/>
@@ -23581,7 +23552,7 @@
       <c r="E197" s="1">
         <v>38400</v>
       </c>
-      <c r="F197" s="3">
+      <c r="F197">
         <v>36.78</v>
       </c>
       <c r="G197" s="2">
@@ -23600,7 +23571,7 @@
         <v>1170.56</v>
       </c>
       <c r="L197">
-        <v>1768.35</v>
+        <v>1766.56</v>
       </c>
       <c r="O197" s="2"/>
       <c r="P197" s="2"/>
@@ -23621,7 +23592,7 @@
       <c r="E198" s="1">
         <v>38488</v>
       </c>
-      <c r="F198" s="3">
+      <c r="F198">
         <v>34.74</v>
       </c>
       <c r="G198" s="2">
@@ -23640,7 +23611,7 @@
         <v>1150.71</v>
       </c>
       <c r="L198">
-        <v>1764.06</v>
+        <v>1762.27</v>
       </c>
       <c r="O198" s="2"/>
       <c r="P198" s="2"/>
@@ -23661,7 +23632,7 @@
       <c r="E199" s="1">
         <v>38510</v>
       </c>
-      <c r="F199" s="3">
+      <c r="F199">
         <v>35.479999999999997</v>
       </c>
       <c r="G199" s="2">
@@ -23680,7 +23651,7 @@
         <v>1158.08</v>
       </c>
       <c r="L199">
-        <v>1741.34</v>
+        <v>1739.55</v>
       </c>
       <c r="O199" s="2"/>
       <c r="P199" s="2"/>
@@ -23701,7 +23672,7 @@
       <c r="E200" s="1">
         <v>38533</v>
       </c>
-      <c r="F200" s="3">
+      <c r="F200">
         <v>35.32</v>
       </c>
       <c r="G200" s="2">
@@ -23720,7 +23691,7 @@
         <v>1148.8</v>
       </c>
       <c r="L200">
-        <v>1722.78</v>
+        <v>1720.99</v>
       </c>
       <c r="O200" s="2"/>
       <c r="P200" s="2"/>
@@ -23741,7 +23712,7 @@
       <c r="E201" s="1">
         <v>38553</v>
       </c>
-      <c r="F201" s="3">
+      <c r="F201">
         <v>35.159999999999997</v>
       </c>
       <c r="G201" s="2">
@@ -23760,7 +23731,7 @@
         <v>1171.83</v>
       </c>
       <c r="L201">
-        <v>1711.23</v>
+        <v>1709.44</v>
       </c>
       <c r="O201" s="2"/>
       <c r="P201" s="2"/>
@@ -23781,7 +23752,7 @@
       <c r="E202" s="1">
         <v>38573</v>
       </c>
-      <c r="F202" s="3">
+      <c r="F202">
         <v>35.03</v>
       </c>
       <c r="G202" s="2">
@@ -23800,7 +23771,7 @@
         <v>1166.55</v>
       </c>
       <c r="L202">
-        <v>1700.67</v>
+        <v>1698.88</v>
       </c>
       <c r="O202" s="2"/>
       <c r="P202" s="2"/>
@@ -23821,7 +23792,7 @@
       <c r="E203" s="1">
         <v>38621</v>
       </c>
-      <c r="F203" s="3">
+      <c r="F203">
         <v>33.92</v>
       </c>
       <c r="G203" s="2">
@@ -23840,7 +23811,7 @@
         <v>1149.06</v>
       </c>
       <c r="L203">
-        <v>1670.97</v>
+        <v>1669.18</v>
       </c>
       <c r="O203" s="2"/>
       <c r="P203" s="2"/>
@@ -23861,7 +23832,7 @@
       <c r="E204" s="1">
         <v>38736</v>
       </c>
-      <c r="F204" s="3">
+      <c r="F204">
         <v>39.06</v>
       </c>
       <c r="G204" s="2">
@@ -23880,7 +23851,7 @@
         <v>1146.0899999999999</v>
       </c>
       <c r="L204">
-        <v>1813.86</v>
+        <v>1812.07</v>
       </c>
       <c r="O204" s="2"/>
       <c r="P204" s="2"/>
@@ -23901,7 +23872,7 @@
       <c r="E205" s="1">
         <v>38757</v>
       </c>
-      <c r="F205" s="3">
+      <c r="F205">
         <v>39.770000000000003</v>
       </c>
       <c r="G205" s="2">
@@ -23920,7 +23891,7 @@
         <v>1156.52</v>
       </c>
       <c r="L205">
-        <v>1810.67</v>
+        <v>1808.88</v>
       </c>
       <c r="O205" s="2"/>
       <c r="P205" s="2"/>
@@ -23941,7 +23912,7 @@
       <c r="E206" s="1">
         <v>38855</v>
       </c>
-      <c r="F206" s="3">
+      <c r="F206">
         <v>42.74</v>
       </c>
       <c r="G206" s="2">
@@ -23960,7 +23931,7 @@
         <v>1157.68</v>
       </c>
       <c r="L206">
-        <v>1892.45</v>
+        <v>1890.66</v>
       </c>
       <c r="O206" s="2"/>
       <c r="P206" s="2"/>
@@ -23981,7 +23952,7 @@
       <c r="E207" s="1">
         <v>38916</v>
       </c>
-      <c r="F207" s="3">
+      <c r="F207">
         <v>40.71</v>
       </c>
       <c r="G207" s="2">
@@ -24000,7 +23971,7 @@
         <v>1157.49</v>
       </c>
       <c r="L207">
-        <v>1834.13</v>
+        <v>1832.34</v>
       </c>
       <c r="O207" s="2"/>
       <c r="P207" s="2"/>
@@ -24021,7 +23992,7 @@
       <c r="E208" s="1">
         <v>39014</v>
       </c>
-      <c r="F208" s="3">
+      <c r="F208">
         <v>47.14</v>
       </c>
       <c r="G208" s="2">
@@ -24040,7 +24011,7 @@
         <v>1160.46</v>
       </c>
       <c r="L208">
-        <v>1946.45</v>
+        <v>1944.66</v>
       </c>
       <c r="O208" s="2"/>
       <c r="P208" s="2"/>
@@ -24061,7 +24032,7 @@
       <c r="E209" s="1">
         <v>39022</v>
       </c>
-      <c r="F209" s="3">
+      <c r="F209">
         <v>46.93</v>
       </c>
       <c r="G209" s="2">
@@ -24080,7 +24051,7 @@
         <v>1194.25</v>
       </c>
       <c r="L209">
-        <v>1925.45</v>
+        <v>1923.66</v>
       </c>
       <c r="O209" s="2"/>
       <c r="P209" s="2"/>
@@ -24101,7 +24072,7 @@
       <c r="E210" s="1">
         <v>39049</v>
       </c>
-      <c r="F210" s="3">
+      <c r="F210">
         <v>46.2</v>
       </c>
       <c r="G210" s="2">
@@ -24120,7 +24091,7 @@
         <v>1190.25</v>
       </c>
       <c r="L210">
-        <v>1890.2</v>
+        <v>1888.41</v>
       </c>
       <c r="O210" s="2"/>
       <c r="P210" s="2"/>
@@ -24141,7 +24112,7 @@
       <c r="E211" s="1">
         <v>39141</v>
       </c>
-      <c r="F211" s="3">
+      <c r="F211">
         <v>49.39</v>
       </c>
       <c r="G211" s="2">
@@ -24160,7 +24131,7 @@
         <v>1142.4000000000001</v>
       </c>
       <c r="L211">
-        <v>1933.16</v>
+        <v>1931.37</v>
       </c>
       <c r="O211" s="2"/>
       <c r="P211" s="2"/>
@@ -24181,7 +24152,7 @@
       <c r="E212" s="1">
         <v>39225</v>
       </c>
-      <c r="F212" s="3">
+      <c r="F212">
         <v>51.99</v>
       </c>
       <c r="G212" s="2">
@@ -24200,7 +24171,7 @@
         <v>1161.1199999999999</v>
       </c>
       <c r="L212">
-        <v>2019.8</v>
+        <v>2018.01</v>
       </c>
       <c r="O212" s="2"/>
       <c r="P212" s="2"/>
@@ -24221,7 +24192,7 @@
       <c r="E213" s="1">
         <v>39283</v>
       </c>
-      <c r="F213" s="3">
+      <c r="F213">
         <v>47.56</v>
       </c>
       <c r="G213" s="2">
@@ -24240,7 +24211,7 @@
         <v>1198.08</v>
       </c>
       <c r="L213">
-        <v>1963.16</v>
+        <v>1961.37</v>
       </c>
       <c r="O213" s="2"/>
       <c r="P213" s="2"/>
@@ -24261,7 +24232,7 @@
       <c r="E214" s="1">
         <v>39324</v>
       </c>
-      <c r="F214" s="3">
+      <c r="F214">
         <v>43.97</v>
       </c>
       <c r="G214" s="2">
@@ -24280,7 +24251,7 @@
         <v>1155</v>
       </c>
       <c r="L214">
-        <v>1907.41</v>
+        <v>1905.62</v>
       </c>
       <c r="O214" s="2"/>
       <c r="P214" s="2"/>
@@ -24301,7 +24272,7 @@
       <c r="E215" s="1">
         <v>39371</v>
       </c>
-      <c r="F215" s="3">
+      <c r="F215">
         <v>45.11</v>
       </c>
       <c r="G215" s="2">
@@ -24320,7 +24291,7 @@
         <v>1184.04</v>
       </c>
       <c r="L215">
-        <v>1896.23</v>
+        <v>1894.44</v>
       </c>
       <c r="O215" s="2"/>
       <c r="P215" s="2"/>
@@ -24341,7 +24312,7 @@
       <c r="E216" s="1">
         <v>39387</v>
       </c>
-      <c r="F216" s="3">
+      <c r="F216">
         <v>44.32</v>
       </c>
       <c r="G216" s="2">
@@ -24360,7 +24331,7 @@
         <v>1164</v>
       </c>
       <c r="L216">
-        <v>1840.23</v>
+        <v>1838.44</v>
       </c>
       <c r="O216" s="2"/>
       <c r="P216" s="2"/>
@@ -24381,7 +24352,7 @@
       <c r="E217" s="1">
         <v>39437</v>
       </c>
-      <c r="F217" s="3">
+      <c r="F217">
         <v>44.11</v>
       </c>
       <c r="G217" s="2">
@@ -24400,7 +24371,7 @@
         <v>1175.46</v>
       </c>
       <c r="L217">
-        <v>1811.63</v>
+        <v>1809.84</v>
       </c>
       <c r="O217" s="2"/>
       <c r="P217" s="2"/>
@@ -24421,7 +24392,7 @@
       <c r="E218" s="1">
         <v>39492</v>
       </c>
-      <c r="F218" s="3">
+      <c r="F218">
         <v>42.61</v>
       </c>
       <c r="G218" s="2">
@@ -24440,7 +24411,7 @@
         <v>1178.28</v>
       </c>
       <c r="L218">
-        <v>1783.82</v>
+        <v>1782.03</v>
       </c>
       <c r="O218" s="2"/>
       <c r="P218" s="2"/>
@@ -24461,7 +24432,7 @@
       <c r="E219" s="1">
         <v>39553</v>
       </c>
-      <c r="F219" s="3">
+      <c r="F219">
         <v>42.12</v>
       </c>
       <c r="G219" s="2">
@@ -24480,7 +24451,7 @@
         <v>1149.25</v>
       </c>
       <c r="L219">
-        <v>1687.57</v>
+        <v>1685.78</v>
       </c>
       <c r="O219" s="2"/>
       <c r="P219" s="2"/>
@@ -24501,7 +24472,7 @@
       <c r="E220" s="1">
         <v>39587</v>
       </c>
-      <c r="F220" s="3">
+      <c r="F220">
         <v>45.99</v>
       </c>
       <c r="G220" s="2">
@@ -24520,7 +24491,7 @@
         <v>1130.75</v>
       </c>
       <c r="L220">
-        <v>1706.57</v>
+        <v>1704.78</v>
       </c>
       <c r="O220" s="2"/>
       <c r="P220" s="2"/>
@@ -24541,7 +24512,7 @@
       <c r="E221" s="1">
         <v>39675</v>
       </c>
-      <c r="F221" s="3">
+      <c r="F221">
         <v>38.07</v>
       </c>
       <c r="G221" s="2">
@@ -24560,7 +24531,7 @@
         <v>1159.5</v>
       </c>
       <c r="L221">
-        <v>1689.17</v>
+        <v>1687.38</v>
       </c>
       <c r="O221" s="2"/>
       <c r="P221" s="2"/>
@@ -24581,7 +24552,7 @@
       <c r="E222" s="1">
         <v>39730</v>
       </c>
-      <c r="F222" s="3">
+      <c r="F222">
         <v>36.68</v>
       </c>
       <c r="G222" s="2">
@@ -24600,7 +24571,7 @@
         <v>1137.3</v>
       </c>
       <c r="L222">
-        <v>1652.27</v>
+        <v>1650.48</v>
       </c>
       <c r="O222" s="2"/>
       <c r="P222" s="2"/>
@@ -24621,7 +24592,7 @@
       <c r="E223" s="1">
         <v>39762</v>
       </c>
-      <c r="F223" s="3">
+      <c r="F223">
         <v>36.409999999999997</v>
       </c>
       <c r="G223" s="2">
@@ -24640,7 +24611,7 @@
         <v>1137.3800000000001</v>
       </c>
       <c r="L223">
-        <v>1570.78</v>
+        <v>1568.99</v>
       </c>
       <c r="O223" s="2"/>
       <c r="P223" s="2"/>
@@ -24661,7 +24632,7 @@
       <c r="E224" s="1">
         <v>39799</v>
       </c>
-      <c r="F224" s="3">
+      <c r="F224">
         <v>31.86</v>
       </c>
       <c r="G224" s="2">
@@ -24680,7 +24651,7 @@
         <v>1154.6400000000001</v>
       </c>
       <c r="L224">
-        <v>1499.38</v>
+        <v>1497.59</v>
       </c>
       <c r="O224" s="2"/>
       <c r="P224" s="2"/>
@@ -24701,7 +24672,7 @@
       <c r="E225" s="1">
         <v>39806</v>
       </c>
-      <c r="F225" s="3">
+      <c r="F225">
         <v>29.85</v>
       </c>
       <c r="G225" s="2">
@@ -24720,7 +24691,7 @@
         <v>1147.98</v>
       </c>
       <c r="L225">
-        <v>1485.7</v>
+        <v>1483.91</v>
       </c>
       <c r="O225" s="2"/>
       <c r="P225" s="2"/>
@@ -24741,7 +24712,7 @@
       <c r="E226" s="1">
         <v>39861</v>
       </c>
-      <c r="F226" s="3">
+      <c r="F226">
         <v>21.65</v>
       </c>
       <c r="G226" s="2">
@@ -24760,7 +24731,7 @@
         <v>1145.76</v>
       </c>
       <c r="L226">
-        <v>1249.24</v>
+        <v>1247.45</v>
       </c>
       <c r="O226" s="2"/>
       <c r="P226" s="2"/>
@@ -24781,7 +24752,7 @@
       <c r="E227" s="1">
         <v>39968</v>
       </c>
-      <c r="F227" s="3">
+      <c r="F227">
         <v>35.35</v>
       </c>
       <c r="G227" s="2">
@@ -24800,7 +24771,7 @@
         <v>1108.32</v>
       </c>
       <c r="L227">
-        <v>1837.72</v>
+        <v>1835.93</v>
       </c>
       <c r="O227" s="2"/>
       <c r="P227" s="2"/>
@@ -24821,7 +24792,7 @@
       <c r="E228" s="1">
         <v>40060</v>
       </c>
-      <c r="F228" s="3">
+      <c r="F228">
         <v>42.34</v>
       </c>
       <c r="G228" s="2">
@@ -24840,7 +24811,7 @@
         <v>1160.32</v>
       </c>
       <c r="L228">
-        <v>2032.28</v>
+        <v>2030.49</v>
       </c>
       <c r="O228" s="2"/>
       <c r="P228" s="2"/>
@@ -24861,7 +24832,7 @@
       <c r="E229" s="1">
         <v>40088</v>
       </c>
-      <c r="F229" s="3">
+      <c r="F229">
         <v>41.86</v>
       </c>
       <c r="G229" s="2">
@@ -24880,7 +24851,7 @@
         <v>1161.54</v>
       </c>
       <c r="L229">
-        <v>2000.96</v>
+        <v>1999.17</v>
       </c>
       <c r="O229" s="2"/>
       <c r="P229" s="2"/>
@@ -24901,7 +24872,7 @@
       <c r="E230" s="1">
         <v>40113</v>
       </c>
-      <c r="F230" s="3">
+      <c r="F230">
         <v>43.9</v>
       </c>
       <c r="G230" s="2">
@@ -24920,7 +24891,7 @@
         <v>1177.8</v>
       </c>
       <c r="L230">
-        <v>1964.56</v>
+        <v>1962.77</v>
       </c>
       <c r="O230" s="2"/>
       <c r="P230" s="2"/>
@@ -24941,7 +24912,7 @@
       <c r="E231" s="1">
         <v>40200</v>
       </c>
-      <c r="F231" s="3">
+      <c r="F231">
         <v>39.159999999999997</v>
       </c>
       <c r="G231" s="2">
@@ -24960,7 +24931,7 @@
         <v>1168.1600000000001</v>
       </c>
       <c r="L231">
-        <v>1892.88</v>
+        <v>1891.09</v>
       </c>
       <c r="O231" s="2"/>
       <c r="P231" s="2"/>
@@ -24981,7 +24952,7 @@
       <c r="E232" s="1">
         <v>40291</v>
       </c>
-      <c r="F232" s="3">
+      <c r="F232">
         <v>44.94</v>
       </c>
       <c r="G232" s="2">
@@ -25000,7 +24971,7 @@
         <v>1184.6500000000001</v>
       </c>
       <c r="L232">
-        <v>2011.49</v>
+        <v>2009.7</v>
       </c>
       <c r="O232" s="2"/>
       <c r="P232" s="2"/>
@@ -25021,7 +24992,7 @@
       <c r="E233" s="1">
         <v>40358</v>
       </c>
-      <c r="F233" s="3">
+      <c r="F233">
         <v>37.06</v>
       </c>
       <c r="G233" s="2">
@@ -25040,7 +25011,7 @@
         <v>1166.0999999999999</v>
       </c>
       <c r="L233">
-        <v>1957.19</v>
+        <v>1955.4</v>
       </c>
       <c r="O233" s="2"/>
       <c r="P233" s="2"/>
@@ -25061,7 +25032,7 @@
       <c r="E234" s="1">
         <v>40401</v>
       </c>
-      <c r="F234" s="3">
+      <c r="F234">
         <v>37.770000000000003</v>
       </c>
       <c r="G234" s="2">
@@ -25080,7 +25051,7 @@
         <v>1175.7</v>
       </c>
       <c r="L234">
-        <v>1914.59</v>
+        <v>1912.8</v>
       </c>
       <c r="O234" s="2"/>
       <c r="P234" s="2"/>
@@ -25101,7 +25072,7 @@
       <c r="E235" s="1">
         <v>40451</v>
       </c>
-      <c r="F235" s="3">
+      <c r="F235">
         <v>38.06</v>
       </c>
       <c r="G235" s="2">
@@ -25120,7 +25091,7 @@
         <v>1173.5999999999999</v>
       </c>
       <c r="L235">
-        <v>1882.79</v>
+        <v>1881</v>
       </c>
       <c r="O235" s="2"/>
       <c r="P235" s="2"/>
@@ -25141,7 +25112,7 @@
       <c r="E236" s="1">
         <v>40464</v>
       </c>
-      <c r="F236" s="3">
+      <c r="F236">
         <v>39.840000000000003</v>
       </c>
       <c r="G236" s="2">
@@ -25160,7 +25131,7 @@
         <v>1171.5999999999999</v>
       </c>
       <c r="L236">
-        <v>1866.55</v>
+        <v>1864.76</v>
       </c>
       <c r="O236" s="2"/>
       <c r="P236" s="2"/>
@@ -25181,7 +25152,7 @@
       <c r="E237" s="1">
         <v>40506</v>
       </c>
-      <c r="F237" s="3">
+      <c r="F237">
         <v>38.159999999999997</v>
       </c>
       <c r="G237" s="2">
@@ -25200,7 +25171,7 @@
         <v>1146.32</v>
       </c>
       <c r="L237">
-        <v>1788.71</v>
+        <v>1786.92</v>
       </c>
       <c r="O237" s="2"/>
       <c r="P237" s="2"/>
@@ -25221,7 +25192,7 @@
       <c r="E238" s="1">
         <v>40606</v>
       </c>
-      <c r="F238" s="3">
+      <c r="F238">
         <v>45.52</v>
       </c>
       <c r="G238" s="2">
@@ -25240,7 +25211,7 @@
         <v>1177.5</v>
       </c>
       <c r="L238">
-        <v>1976.81</v>
+        <v>1975.02</v>
       </c>
       <c r="O238" s="2"/>
       <c r="P238" s="2"/>
@@ -25261,7 +25232,7 @@
       <c r="E239" s="1">
         <v>40651</v>
       </c>
-      <c r="F239" s="3">
+      <c r="F239">
         <v>43.96</v>
       </c>
       <c r="G239" s="2">
@@ -25280,7 +25251,7 @@
         <v>1194.96</v>
       </c>
       <c r="L239">
-        <v>1924.81</v>
+        <v>1923.02</v>
       </c>
       <c r="O239" s="2"/>
       <c r="P239" s="2"/>
@@ -25301,7 +25272,7 @@
       <c r="E240" s="1">
         <v>40735</v>
       </c>
-      <c r="F240" s="3">
+      <c r="F240">
         <v>39.43</v>
       </c>
       <c r="G240" s="2">
@@ -25320,7 +25291,7 @@
         <v>1176.24</v>
       </c>
       <c r="L240">
-        <v>1892.04</v>
+        <v>1890.25</v>
       </c>
       <c r="O240" s="2"/>
       <c r="P240" s="2"/>
@@ -25341,7 +25312,7 @@
       <c r="E241" s="1">
         <v>40757</v>
       </c>
-      <c r="F241" s="3">
+      <c r="F241">
         <v>39.840000000000003</v>
       </c>
       <c r="G241" s="2">
@@ -25360,7 +25331,7 @@
         <v>1184.1199999999999</v>
       </c>
       <c r="L241">
-        <v>1823.44</v>
+        <v>1821.65</v>
       </c>
       <c r="O241" s="2"/>
       <c r="P241" s="2"/>
@@ -25381,7 +25352,7 @@
       <c r="E242" s="1">
         <v>40792</v>
       </c>
-      <c r="F242" s="3">
+      <c r="F242">
         <v>33.44</v>
       </c>
       <c r="G242" s="2">
@@ -25400,7 +25371,7 @@
         <v>1161.5999999999999</v>
       </c>
       <c r="L242">
-        <v>1731.92</v>
+        <v>1730.13</v>
       </c>
       <c r="O242" s="2"/>
       <c r="P242" s="2"/>
@@ -25421,7 +25392,7 @@
       <c r="E243" s="1">
         <v>40861</v>
       </c>
-      <c r="F243" s="3">
+      <c r="F243">
         <v>32.549999999999997</v>
       </c>
       <c r="G243" s="2">
@@ -25440,7 +25411,7 @@
         <v>1162.8</v>
       </c>
       <c r="L243">
-        <v>1740.92</v>
+        <v>1739.13</v>
       </c>
       <c r="O243" s="2"/>
       <c r="P243" s="2"/>
@@ -25461,7 +25432,7 @@
       <c r="E244" s="1">
         <v>41010</v>
       </c>
-      <c r="F244" s="3">
+      <c r="F244">
         <v>44.01</v>
       </c>
       <c r="G244" s="2">
@@ -25480,7 +25451,7 @@
         <v>1163.05</v>
       </c>
       <c r="L244">
-        <v>2118.2199999999998</v>
+        <v>2116.4299999999998</v>
       </c>
       <c r="O244" s="2"/>
       <c r="P244" s="2"/>
@@ -25501,7 +25472,7 @@
       <c r="E245" s="1">
         <v>41100</v>
       </c>
-      <c r="F245" s="3">
+      <c r="F245">
         <v>34.25</v>
       </c>
       <c r="G245" s="2">
@@ -25520,7 +25491,7 @@
         <v>1191.02</v>
       </c>
       <c r="L245">
-        <v>2091.6999999999998</v>
+        <v>2089.91</v>
       </c>
       <c r="O245" s="2"/>
       <c r="P245" s="2"/>
@@ -25541,7 +25512,7 @@
       <c r="E246" s="1">
         <v>41208</v>
       </c>
-      <c r="F246" s="3">
+      <c r="F246">
         <v>41.16</v>
       </c>
       <c r="G246" s="2">
@@ -25560,7 +25531,7 @@
         <v>1180.48</v>
       </c>
       <c r="L246">
-        <v>2228.34</v>
+        <v>2226.5500000000002</v>
       </c>
       <c r="O246" s="2"/>
       <c r="P246" s="2"/>
@@ -25581,7 +25552,7 @@
       <c r="E247" s="1">
         <v>41221</v>
       </c>
-      <c r="F247" s="3">
+      <c r="F247">
         <v>40.4</v>
       </c>
       <c r="G247" s="2">
@@ -25600,7 +25571,7 @@
         <v>1199.52</v>
       </c>
       <c r="L247">
-        <v>2160.02</v>
+        <v>2158.23</v>
       </c>
       <c r="O247" s="2"/>
       <c r="P247" s="2"/>
@@ -25621,7 +25592,7 @@
       <c r="E248" s="1">
         <v>41354</v>
       </c>
-      <c r="F248" s="3">
+      <c r="F248">
         <v>48.35</v>
       </c>
       <c r="G248" s="2">
@@ -25640,7 +25611,7 @@
         <v>1194.8</v>
       </c>
       <c r="L248">
-        <v>2367.37</v>
+        <v>2365.58</v>
       </c>
       <c r="O248" s="2"/>
       <c r="P248" s="2"/>
@@ -25661,7 +25632,7 @@
       <c r="E249" s="1">
         <v>41381</v>
       </c>
-      <c r="F249" s="3">
+      <c r="F249">
         <v>46.79</v>
       </c>
       <c r="G249" s="2">
@@ -25680,7 +25651,7 @@
         <v>1225.25</v>
       </c>
       <c r="L249">
-        <v>2311.87</v>
+        <v>2310.08</v>
       </c>
       <c r="O249" s="2"/>
       <c r="P249" s="2"/>
@@ -25701,7 +25672,7 @@
       <c r="E250" s="1">
         <v>41400</v>
       </c>
-      <c r="F250" s="3">
+      <c r="F250">
         <v>48.18</v>
       </c>
       <c r="G250" s="2">
@@ -25720,7 +25691,7 @@
         <v>1222</v>
       </c>
       <c r="L250">
-        <v>2294.37</v>
+        <v>2292.58</v>
       </c>
       <c r="O250" s="2"/>
       <c r="P250" s="2"/>
@@ -25741,7 +25712,7 @@
       <c r="E251" s="1">
         <v>41445</v>
       </c>
-      <c r="F251" s="3">
+      <c r="F251">
         <v>52.48</v>
       </c>
       <c r="G251" s="2">
@@ -25760,7 +25731,7 @@
         <v>1194.24</v>
       </c>
       <c r="L251">
-        <v>2359.65</v>
+        <v>2357.86</v>
       </c>
       <c r="O251" s="2"/>
       <c r="P251" s="2"/>
@@ -25781,7 +25752,7 @@
       <c r="E252" s="1">
         <v>41495</v>
       </c>
-      <c r="F252" s="3">
+      <c r="F252">
         <v>54.52</v>
       </c>
       <c r="G252" s="2">
@@ -25800,7 +25771,7 @@
         <v>1203.4000000000001</v>
       </c>
       <c r="L252">
-        <v>2355.69</v>
+        <v>2353.9</v>
       </c>
       <c r="O252" s="2"/>
       <c r="P252" s="2"/>
@@ -25821,7 +25792,7 @@
       <c r="E253" s="1">
         <v>41542</v>
       </c>
-      <c r="F253" s="3">
+      <c r="F253">
         <v>51.7</v>
       </c>
       <c r="G253" s="2">
@@ -25840,7 +25811,7 @@
         <v>1224.98</v>
       </c>
       <c r="L253">
-        <v>2319.81</v>
+        <v>2318.02</v>
       </c>
       <c r="O253" s="2"/>
       <c r="P253" s="2"/>
@@ -25861,7 +25832,7 @@
       <c r="E254" s="1">
         <v>41578</v>
       </c>
-      <c r="F254" s="3">
+      <c r="F254">
         <v>51.54</v>
       </c>
       <c r="G254" s="2">
@@ -25880,7 +25851,7 @@
         <v>1188</v>
       </c>
       <c r="L254">
-        <v>2265.69</v>
+        <v>2263.9</v>
       </c>
       <c r="O254" s="2"/>
       <c r="P254" s="2"/>
@@ -25901,7 +25872,7 @@
       <c r="E255" s="1">
         <v>41625</v>
       </c>
-      <c r="F255" s="3">
+      <c r="F255">
         <v>55.72</v>
       </c>
       <c r="G255" s="2">
@@ -25920,7 +25891,7 @@
         <v>1190.2</v>
       </c>
       <c r="L255">
-        <v>2301.33</v>
+        <v>2299.54</v>
       </c>
       <c r="O255" s="2"/>
       <c r="P255" s="2"/>
@@ -25941,7 +25912,7 @@
       <c r="E256" s="1">
         <v>41662</v>
       </c>
-      <c r="F256" s="3">
+      <c r="F256">
         <v>56.47</v>
       </c>
       <c r="G256" s="2">
@@ -25960,7 +25931,7 @@
         <v>1201.83</v>
       </c>
       <c r="L256">
-        <v>2285.37</v>
+        <v>2283.58</v>
       </c>
       <c r="O256" s="2"/>
       <c r="P256" s="2"/>
@@ -25981,7 +25952,7 @@
       <c r="E257" s="1">
         <v>41715</v>
       </c>
-      <c r="F257" s="3">
+      <c r="F257">
         <v>57.58</v>
       </c>
       <c r="G257" s="2">
@@ -26000,7 +25971,7 @@
         <v>1207.92</v>
       </c>
       <c r="L257">
-        <v>2286.63</v>
+        <v>2284.84</v>
       </c>
       <c r="O257" s="2"/>
       <c r="P257" s="2"/>
@@ -26021,7 +25992,7 @@
       <c r="E258" s="1">
         <v>41739</v>
       </c>
-      <c r="F258" s="3">
+      <c r="F258">
         <v>57.4</v>
       </c>
       <c r="G258" s="2">
@@ -26040,7 +26011,7 @@
         <v>1202.2</v>
       </c>
       <c r="L258">
-        <v>2232.4299999999998</v>
+        <v>2230.64</v>
       </c>
       <c r="O258" s="2"/>
       <c r="P258" s="2"/>
@@ -26061,7 +26032,7 @@
       <c r="E259" s="1">
         <v>41828</v>
       </c>
-      <c r="F259" s="3">
+      <c r="F259">
         <v>55.76</v>
       </c>
       <c r="G259" s="2">
@@ -26080,7 +26051,7 @@
         <v>1219.9000000000001</v>
       </c>
       <c r="L259">
-        <v>2239.25</v>
+        <v>2237.46</v>
       </c>
       <c r="O259" s="2"/>
       <c r="P259" s="2"/>
@@ -26101,7 +26072,7 @@
       <c r="E260" s="1">
         <v>41856</v>
       </c>
-      <c r="F260" s="3">
+      <c r="F260">
         <v>56.06</v>
       </c>
       <c r="G260" s="2">
@@ -26120,7 +26091,7 @@
         <v>1215.06</v>
       </c>
       <c r="L260">
-        <v>2201.4499999999998</v>
+        <v>2199.66</v>
       </c>
       <c r="O260" s="2"/>
       <c r="P260" s="2"/>
@@ -26141,7 +26112,7 @@
       <c r="E261" s="1">
         <v>41914</v>
       </c>
-      <c r="F261" s="3">
+      <c r="F261">
         <v>58.84</v>
       </c>
       <c r="G261" s="2">
@@ -26160,7 +26131,7 @@
         <v>1169.8</v>
       </c>
       <c r="L261">
-        <v>2208.4499999999998</v>
+        <v>2206.66</v>
       </c>
       <c r="O261" s="2"/>
       <c r="P261" s="2"/>
@@ -26181,7 +26152,7 @@
       <c r="E262" s="1">
         <v>41974</v>
       </c>
-      <c r="F262" s="3">
+      <c r="F262">
         <v>60</v>
       </c>
       <c r="G262" s="2">
@@ -26200,7 +26171,7 @@
         <v>1185.8</v>
       </c>
       <c r="L262">
-        <v>2222.65</v>
+        <v>2220.86</v>
       </c>
       <c r="O262" s="2"/>
       <c r="P262" s="2"/>
@@ -26221,7 +26192,7 @@
       <c r="E263" s="1">
         <v>41988</v>
       </c>
-      <c r="F263" s="3">
+      <c r="F263">
         <v>59.16</v>
       </c>
       <c r="G263" s="2">
@@ -26240,7 +26211,7 @@
         <v>1169.26</v>
       </c>
       <c r="L263">
-        <v>2177.4299999999998</v>
+        <v>2175.64</v>
       </c>
       <c r="O263" s="2"/>
       <c r="P263" s="2"/>
@@ -26261,7 +26232,7 @@
       <c r="E264" s="1">
         <v>42011</v>
       </c>
-      <c r="F264" s="3">
+      <c r="F264">
         <v>59.07</v>
       </c>
       <c r="G264" s="2">
@@ -26280,7 +26251,7 @@
         <v>1187.1199999999999</v>
       </c>
       <c r="L264">
-        <v>2112.64</v>
+        <v>2110.85</v>
       </c>
       <c r="O264" s="2"/>
       <c r="P264" s="2"/>
@@ -26301,7 +26272,7 @@
       <c r="E265" s="1">
         <v>42088</v>
       </c>
-      <c r="F265" s="3">
+      <c r="F265">
         <v>59.61</v>
       </c>
       <c r="G265" s="2">
@@ -26320,7 +26291,7 @@
         <v>1169.2</v>
       </c>
       <c r="L265">
-        <v>2135.64</v>
+        <v>2133.85</v>
       </c>
       <c r="O265" s="2"/>
       <c r="P265" s="2"/>
@@ -26341,7 +26312,7 @@
       <c r="E266" s="1">
         <v>42191</v>
       </c>
-      <c r="F266" s="3">
+      <c r="F266">
         <v>67.33</v>
       </c>
       <c r="G266" s="2">
@@ -26360,7 +26331,7 @@
         <v>1167.93</v>
       </c>
       <c r="L266">
-        <v>2246.98</v>
+        <v>2245.19</v>
       </c>
       <c r="O266" s="2"/>
       <c r="P266" s="2"/>
@@ -26381,7 +26352,7 @@
       <c r="E267" s="1">
         <v>42227</v>
       </c>
-      <c r="F267" s="3">
+      <c r="F267">
         <v>68.23</v>
       </c>
       <c r="G267" s="2">
@@ -26400,7 +26371,7 @@
         <v>1182.52</v>
       </c>
       <c r="L267">
-        <v>2224.37</v>
+        <v>2222.58</v>
       </c>
       <c r="O267" s="2"/>
       <c r="P267" s="2"/>
@@ -26421,7 +26392,7 @@
       <c r="E268" s="1">
         <v>42291</v>
       </c>
-      <c r="F268" s="3">
+      <c r="F268">
         <v>59.99</v>
       </c>
       <c r="G268" s="2">
@@ -26440,7 +26411,7 @@
         <v>1180.47</v>
       </c>
       <c r="L268">
-        <v>2183.71</v>
+        <v>2181.92</v>
       </c>
       <c r="O268" s="2"/>
       <c r="P268" s="2"/>
@@ -26461,7 +26432,7 @@
       <c r="E269" s="1">
         <v>42346</v>
       </c>
-      <c r="F269" s="3">
+      <c r="F269">
         <v>65.959999999999994</v>
       </c>
       <c r="G269" s="2">
@@ -26480,7 +26451,7 @@
         <v>1182.18</v>
       </c>
       <c r="L269">
-        <v>2254.77</v>
+        <v>2252.98</v>
       </c>
       <c r="O269" s="2"/>
       <c r="P269" s="2"/>
@@ -26501,7 +26472,7 @@
       <c r="E270" s="1">
         <v>42373</v>
       </c>
-      <c r="F270" s="3">
+      <c r="F270">
         <v>63.62</v>
       </c>
       <c r="G270" s="2">
@@ -26520,7 +26491,7 @@
         <v>1207.26</v>
       </c>
       <c r="L270">
-        <v>2192.67</v>
+        <v>2190.88</v>
       </c>
       <c r="O270" s="2"/>
       <c r="P270" s="2"/>
@@ -26541,7 +26512,7 @@
       <c r="E271" s="1">
         <v>42426</v>
       </c>
-      <c r="F271" s="3">
+      <c r="F271">
         <v>57.54</v>
       </c>
       <c r="G271" s="2">
@@ -26560,7 +26531,7 @@
         <v>1214.01</v>
       </c>
       <c r="L271">
-        <v>2187</v>
+        <v>2185.21</v>
       </c>
       <c r="O271" s="2"/>
       <c r="P271" s="2"/>
@@ -26581,7 +26552,7 @@
       <c r="E272" s="1">
         <v>42465</v>
       </c>
-      <c r="F272" s="3">
+      <c r="F272">
         <v>58.36</v>
       </c>
       <c r="G272" s="2">
@@ -26600,7 +26571,7 @@
         <v>1195.2</v>
       </c>
       <c r="L272">
-        <v>2159</v>
+        <v>2157.21</v>
       </c>
       <c r="O272" s="2"/>
       <c r="P272" s="2"/>
@@ -26621,7 +26592,7 @@
       <c r="E273" s="1">
         <v>42499</v>
       </c>
-      <c r="F273" s="3">
+      <c r="F273">
         <v>61.21</v>
       </c>
       <c r="G273" s="2">
@@ -26640,7 +26611,7 @@
         <v>1189.21</v>
       </c>
       <c r="L273">
-        <v>2132.7800000000002</v>
+        <v>2130.9899999999998</v>
       </c>
       <c r="O273" s="2"/>
       <c r="P273" s="2"/>
@@ -26661,7 +26632,7 @@
       <c r="E274" s="1">
         <v>42535</v>
       </c>
-      <c r="F274" s="3">
+      <c r="F274">
         <v>62.08</v>
       </c>
       <c r="G274" s="2">
@@ -26680,7 +26651,7 @@
         <v>1206.69</v>
       </c>
       <c r="L274">
-        <v>2105.61</v>
+        <v>2103.8200000000002</v>
       </c>
       <c r="O274" s="2"/>
       <c r="P274" s="2"/>
@@ -26701,7 +26672,7 @@
       <c r="E275" s="1">
         <v>42632</v>
       </c>
-      <c r="F275" s="3">
+      <c r="F275">
         <v>66.19</v>
       </c>
       <c r="G275" s="2">
@@ -26720,7 +26691,7 @@
         <v>1200.04</v>
       </c>
       <c r="L275">
-        <v>2163.1799999999998</v>
+        <v>2161.39</v>
       </c>
       <c r="O275" s="2"/>
       <c r="P275" s="2"/>
@@ -26741,7 +26712,7 @@
       <c r="E276" s="1">
         <v>42641</v>
       </c>
-      <c r="F276" s="3">
+      <c r="F276">
         <v>66.709999999999994</v>
       </c>
       <c r="G276" s="2">
@@ -26760,7 +26731,7 @@
         <v>1210.5</v>
       </c>
       <c r="L276">
-        <v>2153.46</v>
+        <v>2151.67</v>
       </c>
       <c r="O276" s="2"/>
       <c r="P276" s="2"/>
@@ -26781,7 +26752,7 @@
       <c r="E277" s="1">
         <v>42752</v>
       </c>
-      <c r="F277" s="3">
+      <c r="F277">
         <v>83.55</v>
       </c>
       <c r="G277" s="2">
@@ -26800,7 +26771,7 @@
         <v>1153.79</v>
       </c>
       <c r="L277">
-        <v>2420.02</v>
+        <v>2418.23</v>
       </c>
       <c r="O277" s="2"/>
       <c r="P277" s="2"/>
@@ -26821,7 +26792,7 @@
       <c r="E278" s="1">
         <v>42768</v>
       </c>
-      <c r="F278" s="3">
+      <c r="F278">
         <v>84.59</v>
       </c>
       <c r="G278" s="2">
@@ -26840,7 +26811,7 @@
         <v>1204.42</v>
       </c>
       <c r="L278">
-        <v>2399.86</v>
+        <v>2398.0700000000002</v>
       </c>
       <c r="O278" s="2"/>
       <c r="P278" s="2"/>
@@ -26861,7 +26832,7 @@
       <c r="E279" s="1">
         <v>42815</v>
       </c>
-      <c r="F279" s="3">
+      <c r="F279">
         <v>87.39</v>
       </c>
       <c r="G279" s="2">
@@ -26880,7 +26851,7 @@
         <v>1214.08</v>
       </c>
       <c r="L279">
-        <v>2409.2399999999998</v>
+        <v>2407.4499999999998</v>
       </c>
       <c r="O279" s="2"/>
       <c r="P279" s="2"/>
@@ -26901,7 +26872,7 @@
       <c r="E280" s="1">
         <v>42873</v>
       </c>
-      <c r="F280" s="3">
+      <c r="F280">
         <v>83.96</v>
       </c>
       <c r="G280" s="2">
@@ -26920,7 +26891,7 @@
         <v>1238.02</v>
       </c>
       <c r="L280">
-        <v>2346.66</v>
+        <v>2344.87</v>
       </c>
       <c r="O280" s="2"/>
       <c r="P280" s="2"/>
@@ -26941,7 +26912,7 @@
       <c r="E281" s="1">
         <v>42963</v>
       </c>
-      <c r="F281" s="3">
+      <c r="F281">
         <v>92.09</v>
       </c>
       <c r="G281" s="2">
@@ -26960,7 +26931,7 @@
         <v>1221.78</v>
       </c>
       <c r="L281">
-        <v>2414.14</v>
+        <v>2412.35</v>
       </c>
       <c r="O281" s="2"/>
       <c r="P281" s="2"/>
@@ -26981,7 +26952,7 @@
       <c r="E282" s="1">
         <v>43049</v>
       </c>
-      <c r="F282" s="3">
+      <c r="F282">
         <v>97.51</v>
       </c>
       <c r="G282" s="2">
@@ -27000,7 +26971,7 @@
         <v>1207.96</v>
       </c>
       <c r="L282">
-        <v>2473.81</v>
+        <v>2472.02</v>
       </c>
       <c r="O282" s="2"/>
       <c r="P282" s="2"/>
@@ -27021,7 +26992,7 @@
       <c r="E283" s="1">
         <v>43139</v>
       </c>
-      <c r="F283" s="3">
+      <c r="F283">
         <v>107.88</v>
       </c>
       <c r="G283" s="2">
@@ -27040,7 +27011,7 @@
         <v>1244.76</v>
       </c>
       <c r="L283">
-        <v>2523.61</v>
+        <v>2521.8200000000002</v>
       </c>
       <c r="O283" s="2"/>
       <c r="P283" s="2"/>
@@ -27061,7 +27032,7 @@
       <c r="E284" s="1">
         <v>43179</v>
       </c>
-      <c r="F284" s="3">
+      <c r="F284">
         <v>114.64</v>
       </c>
       <c r="G284" s="2">
@@ -27080,7 +27051,7 @@
         <v>1146.8</v>
       </c>
       <c r="L284">
-        <v>2523.21</v>
+        <v>2521.42</v>
       </c>
       <c r="O284" s="2"/>
       <c r="P284" s="2"/>
@@ -27101,7 +27072,7 @@
       <c r="E285" s="1">
         <v>43220</v>
       </c>
-      <c r="F285" s="3">
+      <c r="F285">
         <v>108.78</v>
       </c>
       <c r="G285" s="2">
@@ -27120,7 +27091,7 @@
         <v>1220.23</v>
       </c>
       <c r="L285">
-        <v>2499.56</v>
+        <v>2497.77</v>
       </c>
       <c r="O285" s="2"/>
       <c r="P285" s="2"/>
@@ -27141,7 +27112,7 @@
       <c r="E286" s="1">
         <v>43249</v>
       </c>
-      <c r="F286" s="3">
+      <c r="F286">
         <v>105.93</v>
       </c>
       <c r="G286" s="2">
@@ -27160,7 +27131,7 @@
         <v>1142.9000000000001</v>
       </c>
       <c r="L286">
-        <v>2415.96</v>
+        <v>2414.17</v>
       </c>
       <c r="O286" s="2"/>
       <c r="P286" s="2"/>
@@ -27181,7 +27152,7 @@
       <c r="E287" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F287" s="3">
+      <c r="F287">
         <v>113.89</v>
       </c>
       <c r="G287" s="2">
@@ -27200,13 +27171,13 @@
         <v>1169.96</v>
       </c>
       <c r="L287">
-        <v>2498.79</v>
+        <v>2497</v>
       </c>
       <c r="O287" s="2"/>
       <c r="P287" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>